<commit_message>
Update SystemsOverview component with improved data handling and UI enhancements
</commit_message>
<xml_diff>
--- a/public/Project Performance Template.xlsx
+++ b/public/Project Performance Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yahya Chaker\OneDrive\Desktop\Project Performance Review - 01\business-dashboard\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yahya Chaker\OneDrive\Desktop\Project Performance Review - 01\business-dashboard\business-dashboard\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2338451A-653D-47E2-90CA-7721668DEDF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27839A03-46B4-492E-A9E9-E8F13A08A428}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="805" activeTab="7" xr2:uid="{23CBEA3F-BC00-4514-8C1F-F15676C82A9D}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="805" firstSheet="2" activeTab="2" xr2:uid="{23CBEA3F-BC00-4514-8C1F-F15676C82A9D}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Overview" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,11 @@
     <sheet name="WOs" sheetId="8" r:id="rId9"/>
     <sheet name="Services" sheetId="10" r:id="rId10"/>
     <sheet name="Subcontractors" sheetId="11" r:id="rId11"/>
+    <sheet name="Subcontractor Monthly Billing" sheetId="13" r:id="rId12"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId12"/>
     <externalReference r:id="rId13"/>
+    <externalReference r:id="rId14"/>
   </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
@@ -114,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="311" uniqueCount="160">
   <si>
     <t>Project Title</t>
   </si>
@@ -474,9 +475,6 @@
     <t>Subcon-06</t>
   </si>
   <si>
-    <t>Total Value</t>
-  </si>
-  <si>
     <t>Strat Date</t>
   </si>
   <si>
@@ -492,9 +490,6 @@
     <t>Monthly Billing</t>
   </si>
   <si>
-    <t>Monthly Billing Submittal</t>
-  </si>
-  <si>
     <t>*if no amount is added then no invoice is received</t>
   </si>
   <si>
@@ -604,6 +599,24 @@
   </si>
   <si>
     <t>Planned vs. Completed Progress (PPM)</t>
+  </si>
+  <si>
+    <t>Total Contract Value</t>
+  </si>
+  <si>
+    <t>Total Budgeted Vlaue</t>
+  </si>
+  <si>
+    <t>Bill Details</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Subcontractor Monthly Billing Submittal</t>
+  </si>
+  <si>
+    <t>Subcontractors</t>
   </si>
 </sst>
 </file>
@@ -616,7 +629,7 @@
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="mmmm\-yyyy"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -716,6 +729,21 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -755,7 +783,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="86">
+  <borders count="93">
     <border>
       <left/>
       <right/>
@@ -1564,30 +1592,6 @@
       <bottom style="hair">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="hair">
-        <color auto="1"/>
-      </left>
-      <right style="hair">
-        <color auto="1"/>
-      </right>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1650,19 +1654,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="hair">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="hair">
@@ -1848,16 +1839,140 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom style="hair">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="medium">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thick">
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right style="hair">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="hair">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -1866,7 +1981,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="285">
+  <cellXfs count="293">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -2248,18 +2363,9 @@
     </xf>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="52" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="3" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2269,22 +2375,16 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="57" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="58" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="60" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="61" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="44" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="58" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="64" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="3" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="3" fillId="0" borderId="65" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="3" fillId="0" borderId="63" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="3" fillId="0" borderId="47" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="4" fillId="3" borderId="68" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="4" fillId="3" borderId="68" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="4" fillId="3" borderId="69" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="65" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="4" fillId="3" borderId="66" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="4" fillId="3" borderId="66" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="2" fillId="3" borderId="53" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2298,19 +2398,19 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="3" fillId="0" borderId="23" xfId="1" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="3" fillId="0" borderId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -2332,19 +2432,47 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="79" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="78" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="81" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="82" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="77" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="75" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="76" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="4" fillId="3" borderId="33" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="84" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="64" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="62" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="15" fillId="3" borderId="22" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="83" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="84" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="88" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="89" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="90" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="47" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="64" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="2" borderId="78" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="91" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="3" fillId="5" borderId="79" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="80" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="81" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="5" borderId="15" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="42" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="5" borderId="50" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="47" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="64" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2402,16 +2530,16 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="71" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="75" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="72" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="76" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="17" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -2462,35 +2590,57 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="77" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="54" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="62" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="10">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFBDBD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -2544,6 +2694,7 @@
   <colors>
     <mruColors>
       <color rgb="FFFF00FF"/>
+      <color rgb="FFFFBDBD"/>
       <color rgb="FFFF7575"/>
       <color rgb="FFFF9F9F"/>
     </mruColors>
@@ -3050,12 +3201,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="23.4" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A1" s="232" t="s">
+      <c r="A1" s="237" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="233"/>
-      <c r="C1" s="233"/>
-      <c r="D1" s="234"/>
+      <c r="B1" s="238"/>
+      <c r="C1" s="238"/>
+      <c r="D1" s="239"/>
     </row>
     <row r="2" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -3082,7 +3233,7 @@
         <v>7</v>
       </c>
       <c r="D3" s="68" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
@@ -3160,10 +3311,10 @@
   <sheetPr>
     <tabColor rgb="FFFF00FF"/>
   </sheetPr>
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3176,16 +3327,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="268" t="s">
+      <c r="A1" s="273" t="s">
         <v>104</v>
       </c>
-      <c r="B1" s="269"/>
-      <c r="C1" s="269"/>
-      <c r="D1" s="269"/>
-      <c r="E1" s="269"/>
-      <c r="F1" s="269"/>
-      <c r="G1" s="269"/>
-      <c r="H1" s="270"/>
+      <c r="B1" s="274"/>
+      <c r="C1" s="274"/>
+      <c r="D1" s="274"/>
+      <c r="E1" s="274"/>
+      <c r="F1" s="274"/>
+      <c r="G1" s="274"/>
+      <c r="H1" s="275"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="156" t="s">
@@ -3558,6 +3709,21 @@
       <c r="F17" s="129"/>
       <c r="G17" s="129"/>
       <c r="H17" s="153"/>
+    </row>
+    <row r="18" spans="1:8" s="218" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="215"/>
+      <c r="B18" s="216" t="s">
+        <v>37</v>
+      </c>
+      <c r="C18" s="216"/>
+      <c r="D18" s="216"/>
+      <c r="E18" s="216"/>
+      <c r="F18" s="216"/>
+      <c r="G18" s="216"/>
+      <c r="H18" s="217">
+        <f>SUM(H3:H17)</f>
+        <v>20300000</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3587,897 +3753,1030 @@
   <sheetPr>
     <tabColor rgb="FFFF00FF"/>
   </sheetPr>
-  <dimension ref="A1:K35"/>
+  <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.88671875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.21875" style="10" customWidth="1"/>
     <col min="2" max="2" width="21.88671875" style="10" customWidth="1"/>
-    <col min="3" max="10" width="12.88671875" style="10"/>
+    <col min="3" max="8" width="13.109375" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="12.88671875" style="10"/>
     <col min="11" max="11" width="14.33203125" style="10" bestFit="1" customWidth="1"/>
     <col min="12" max="16384" width="12.88671875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="274" t="s">
-        <v>114</v>
-      </c>
-      <c r="B2" s="275"/>
-      <c r="C2" s="167" t="str" cm="1">
+    <row r="1" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="276" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="276"/>
+      <c r="C1" s="276"/>
+      <c r="D1" s="276"/>
+      <c r="E1" s="276"/>
+      <c r="F1" s="276"/>
+      <c r="G1" s="276"/>
+      <c r="H1" s="276"/>
+      <c r="I1" s="276"/>
+      <c r="J1" s="276"/>
+      <c r="K1" s="276"/>
+    </row>
+    <row r="2" spans="1:11" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="279" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" s="280"/>
+      <c r="C2" s="219" t="str" cm="1">
         <f t="array" ref="C2:J2">TRANSPOSE(_xlfn._xlws.FILTER(Services!$B$3:$B$17,Services!$C$3:$C$17="Subcontractor"))</f>
         <v>System 8</v>
       </c>
-      <c r="D2" s="167" t="str">
+      <c r="D2" s="219" t="str">
         <v>System 9</v>
       </c>
-      <c r="E2" s="167" t="str">
+      <c r="E2" s="219" t="str">
         <v>System 10</v>
       </c>
-      <c r="F2" s="167" t="str">
+      <c r="F2" s="219" t="str">
         <v>System 11</v>
       </c>
-      <c r="G2" s="167" t="str">
+      <c r="G2" s="219" t="str">
         <v>System 12</v>
       </c>
-      <c r="H2" s="167" t="str">
+      <c r="H2" s="219" t="str">
         <v>System 13</v>
       </c>
-      <c r="I2" s="167" t="str">
+      <c r="I2" s="219" t="str">
         <v>System 14</v>
       </c>
-      <c r="J2" s="168" t="str">
+      <c r="J2" s="220" t="str">
         <v>System 15</v>
       </c>
-      <c r="K2" s="271" t="s">
+      <c r="K2" s="277" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="276" t="s">
-        <v>115</v>
-      </c>
-      <c r="B3" s="277"/>
-      <c r="C3" s="170" t="str">
+      <c r="A3" s="281" t="s">
+        <v>114</v>
+      </c>
+      <c r="B3" s="282"/>
+      <c r="C3" s="165" t="str">
         <f>_xlfn.XLOOKUP(C2,Services!$B$3:$B$17,Services!$D$3:$D$17)</f>
         <v>Subcon-01</v>
       </c>
-      <c r="D3" s="170" t="str">
+      <c r="D3" s="165" t="str">
         <f>_xlfn.XLOOKUP(D2,Services!$B$3:$B$17,Services!$D$3:$D$17)</f>
         <v>Subcon-02</v>
       </c>
-      <c r="E3" s="170" t="str">
+      <c r="E3" s="165" t="str">
         <f>_xlfn.XLOOKUP(E2,Services!$B$3:$B$17,Services!$D$3:$D$17)</f>
         <v>Subcon-03</v>
       </c>
-      <c r="F3" s="170" t="str">
+      <c r="F3" s="165" t="str">
         <f>_xlfn.XLOOKUP(F2,Services!$B$3:$B$17,Services!$D$3:$D$17)</f>
         <v>Subcon-04</v>
       </c>
-      <c r="G3" s="170" t="str">
+      <c r="G3" s="165" t="str">
         <f>_xlfn.XLOOKUP(G2,Services!$B$3:$B$17,Services!$D$3:$D$17)</f>
         <v>Subcon-05</v>
       </c>
-      <c r="H3" s="170" t="str">
+      <c r="H3" s="165" t="str">
         <f>_xlfn.XLOOKUP(H2,Services!$B$3:$B$17,Services!$D$3:$D$17)</f>
         <v>Subcon-06</v>
       </c>
-      <c r="I3" s="170">
+      <c r="I3" s="165">
         <f>_xlfn.XLOOKUP(I2,Services!$B$3:$B$17,Services!$D$3:$D$17)</f>
         <v>0</v>
       </c>
-      <c r="J3" s="171">
+      <c r="J3" s="166">
         <f>_xlfn.XLOOKUP(J2,Services!$B$3:$B$17,Services!$D$3:$D$17)</f>
         <v>0</v>
       </c>
-      <c r="K3" s="272"/>
-    </row>
-    <row r="4" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="278" t="s">
-        <v>112</v>
-      </c>
-      <c r="B4" s="279"/>
-      <c r="C4" s="173">
+      <c r="K3" s="278"/>
+    </row>
+    <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="289" t="s">
+        <v>155</v>
+      </c>
+      <c r="B4" s="281"/>
+      <c r="C4" s="224">
+        <v>1300000</v>
+      </c>
+      <c r="D4" s="224">
+        <f>3200000</f>
+        <v>3200000</v>
+      </c>
+      <c r="E4" s="224">
+        <v>6000000</v>
+      </c>
+      <c r="F4" s="224">
+        <v>1800000</v>
+      </c>
+      <c r="G4" s="224">
+        <v>7800000</v>
+      </c>
+      <c r="H4" s="224">
+        <v>2200000</v>
+      </c>
+      <c r="I4" s="224"/>
+      <c r="J4" s="225"/>
+      <c r="K4" s="226">
+        <f>SUM(C4:J4)</f>
+        <v>22300000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="283" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" s="284"/>
+      <c r="C5" s="168">
         <f>_xlfn.XLOOKUP(C2,Services!$B$3:$B$17,Services!$H$3:$H$17)</f>
         <v>1500000</v>
       </c>
-      <c r="D4" s="173">
+      <c r="D5" s="168">
         <f>_xlfn.XLOOKUP(D2,Services!$B$3:$B$17,Services!$H$3:$H$17)</f>
         <v>3000000</v>
       </c>
-      <c r="E4" s="173">
+      <c r="E5" s="168">
         <f>_xlfn.XLOOKUP(E2,Services!$B$3:$B$17,Services!$H$3:$H$17)</f>
         <v>5000000</v>
       </c>
-      <c r="F4" s="173">
+      <c r="F5" s="168">
         <f>_xlfn.XLOOKUP(F2,Services!$B$3:$B$17,Services!$H$3:$H$17)</f>
         <v>2000000</v>
       </c>
-      <c r="G4" s="173">
+      <c r="G5" s="168">
         <f>_xlfn.XLOOKUP(G2,Services!$B$3:$B$17,Services!$H$3:$H$17)</f>
         <v>7000000</v>
       </c>
-      <c r="H4" s="173">
+      <c r="H5" s="168">
         <f>_xlfn.XLOOKUP(H2,Services!$B$3:$B$17,Services!$H$3:$H$17)</f>
         <v>1800000</v>
       </c>
-      <c r="I4" s="173">
+      <c r="I5" s="168">
         <f>_xlfn.XLOOKUP(I2,Services!$B$3:$B$17,Services!$H$3:$H$17)</f>
         <v>0</v>
       </c>
-      <c r="J4" s="174">
+      <c r="J5" s="168">
         <f>_xlfn.XLOOKUP(J2,Services!$B$3:$B$17,Services!$H$3:$H$17)</f>
         <v>0</v>
       </c>
-      <c r="K4" s="219">
-        <f>SUM(C4:J4)</f>
+      <c r="K5" s="168">
+        <f>SUM(C5:J5)</f>
         <v>20300000</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="280" t="s">
-        <v>113</v>
-      </c>
-      <c r="B5" s="281"/>
-      <c r="C5" s="175">
+    <row r="6" spans="1:11" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="285" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6" s="286"/>
+      <c r="C6" s="169">
         <f>IF(C3&gt;0,_xlfn.XLOOKUP(C2,Services!$B$3:$B$17,Services!$F$3:$F$17),"")</f>
         <v>45413</v>
       </c>
-      <c r="D5" s="175">
+      <c r="D6" s="169">
         <f>IF(D3&gt;0,_xlfn.XLOOKUP(D2,Services!$B$3:$B$17,Services!$F$3:$F$17),"")</f>
         <v>45414</v>
       </c>
-      <c r="E5" s="175">
+      <c r="E6" s="169">
         <f>IF(E3&gt;0,_xlfn.XLOOKUP(E2,Services!$B$3:$B$17,Services!$F$3:$F$17),"")</f>
         <v>45415</v>
       </c>
-      <c r="F5" s="175">
+      <c r="F6" s="169">
         <f>IF(F3&gt;0,_xlfn.XLOOKUP(F2,Services!$B$3:$B$17,Services!$F$3:$F$17),"")</f>
         <v>45416</v>
       </c>
-      <c r="G5" s="175">
+      <c r="G6" s="169">
         <f>IF(G3&gt;0,_xlfn.XLOOKUP(G2,Services!$B$3:$B$17,Services!$F$3:$F$17),"")</f>
         <v>45417</v>
       </c>
-      <c r="H5" s="175">
+      <c r="H6" s="169">
         <f>IF(H3&gt;0,_xlfn.XLOOKUP(H2,Services!$B$3:$B$17,Services!$F$3:$F$17),"")</f>
         <v>45418</v>
       </c>
-      <c r="I5" s="175" t="str">
+      <c r="I6" s="169" t="str">
         <f>IF(I3&gt;0,_xlfn.XLOOKUP(I2,Services!$B$3:$B$17,Services!$F$3:$F$17),"")</f>
         <v/>
       </c>
-      <c r="J5" s="176" t="str">
+      <c r="J6" s="170" t="str">
         <f>IF(J3&gt;0,_xlfn.XLOOKUP(J2,Services!$B$3:$B$17,Services!$F$3:$F$17),"")</f>
         <v/>
       </c>
-      <c r="K5" s="220"/>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="276" t="s">
+      <c r="K6" s="208"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="281" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="277"/>
-      <c r="C6" s="177">
+      <c r="B7" s="282"/>
+      <c r="C7" s="171">
         <f>IF(C3&gt;0,_xlfn.XLOOKUP(C2,Services!$B$3:$B$17,Services!$G$3:$G$17),"")</f>
         <v>46172</v>
       </c>
-      <c r="D6" s="177">
+      <c r="D7" s="171">
         <f>IF(D3&gt;0,_xlfn.XLOOKUP(D2,Services!$B$3:$B$17,Services!$G$3:$G$17),"")</f>
         <v>46172</v>
       </c>
-      <c r="E6" s="177">
+      <c r="E7" s="171">
         <f>IF(E3&gt;0,_xlfn.XLOOKUP(E2,Services!$B$3:$B$17,Services!$G$3:$G$17),"")</f>
         <v>46172</v>
       </c>
-      <c r="F6" s="177">
+      <c r="F7" s="171">
         <f>IF(F3&gt;0,_xlfn.XLOOKUP(F2,Services!$B$3:$B$17,Services!$G$3:$G$17),"")</f>
         <v>46172</v>
       </c>
-      <c r="G6" s="177">
+      <c r="G7" s="171">
         <f>IF(G3&gt;0,_xlfn.XLOOKUP(G2,Services!$B$3:$B$17,Services!$G$3:$G$17),"")</f>
         <v>46172</v>
       </c>
-      <c r="H6" s="177">
+      <c r="H7" s="171">
         <f>IF(H3&gt;0,_xlfn.XLOOKUP(H2,Services!$B$3:$B$17,Services!$G$3:$G$17),"")</f>
         <v>46172</v>
       </c>
-      <c r="I6" s="177" t="str">
+      <c r="I7" s="171" t="str">
         <f>IF(I3&gt;0,_xlfn.XLOOKUP(I2,Services!$B$3:$B$17,Services!$G$3:$G$17),"")</f>
         <v/>
       </c>
-      <c r="J6" s="178" t="str">
+      <c r="J7" s="172" t="str">
         <f>IF(J3&gt;0,_xlfn.XLOOKUP(J2,Services!$B$3:$B$17,Services!$G$3:$G$17),"")</f>
         <v/>
       </c>
-      <c r="K6" s="221"/>
-    </row>
-    <row r="7" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="278" t="s">
+      <c r="K7" s="209"/>
+    </row>
+    <row r="8" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="283" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8" s="284"/>
+      <c r="C8" s="167">
+        <f>IF(C3&gt;0,DATEDIF(C6,C7,"M"),0)</f>
+        <v>24</v>
+      </c>
+      <c r="D8" s="167">
+        <f t="shared" ref="D8:J8" si="0">IF(D3&gt;0,DATEDIF(D6,D7,"M"),0)</f>
+        <v>24</v>
+      </c>
+      <c r="E8" s="167">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="F8" s="167">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="G8" s="167">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="H8" s="167">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="I8" s="167">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="173">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K8" s="210"/>
+    </row>
+    <row r="9" spans="1:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="287" t="s">
         <v>116</v>
       </c>
-      <c r="B7" s="279"/>
-      <c r="C7" s="172">
-        <f>IF(C3&gt;0,DATEDIF(C5,C6,"M"),0)</f>
-        <v>24</v>
-      </c>
-      <c r="D7" s="172">
-        <f t="shared" ref="D7:J7" si="0">IF(D3&gt;0,DATEDIF(D5,D6,"M"),0)</f>
-        <v>24</v>
-      </c>
-      <c r="E7" s="172">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="F7" s="172">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="G7" s="172">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="H7" s="172">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="I7" s="172">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J7" s="179">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K7" s="222"/>
-    </row>
-    <row r="8" spans="1:11" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="282" t="s">
-        <v>117</v>
-      </c>
-      <c r="B8" s="283"/>
-      <c r="C8" s="180">
-        <f>IF(C7&lt;&gt;0,C4/C7,0)</f>
+      <c r="B9" s="288"/>
+      <c r="C9" s="221">
+        <f>IF(C8&lt;&gt;0,C5/C8,0)</f>
         <v>62500</v>
       </c>
-      <c r="D8" s="180">
-        <f t="shared" ref="D8:J8" si="1">IF(D7&lt;&gt;0,D4/D7,0)</f>
+      <c r="D9" s="221">
+        <f t="shared" ref="D9:J9" si="1">IF(D8&lt;&gt;0,D5/D8,0)</f>
         <v>125000</v>
       </c>
-      <c r="E8" s="180">
+      <c r="E9" s="221">
         <f t="shared" si="1"/>
         <v>208333.33333333334</v>
       </c>
-      <c r="F8" s="180">
+      <c r="F9" s="221">
         <f t="shared" si="1"/>
         <v>83333.333333333328</v>
       </c>
-      <c r="G8" s="180">
+      <c r="G9" s="221">
         <f t="shared" si="1"/>
         <v>291666.66666666669</v>
       </c>
-      <c r="H8" s="180">
+      <c r="H9" s="221">
         <f t="shared" si="1"/>
         <v>75000</v>
       </c>
-      <c r="I8" s="180">
+      <c r="I9" s="221">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J8" s="181">
+      <c r="J9" s="222">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K8" s="223">
-        <f>SUM(C8:J8)</f>
+      <c r="K9" s="223">
+        <f>SUM(C9:J9)</f>
         <v>845833.33333333337</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K9" s="224"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" s="284" t="s">
-        <v>118</v>
-      </c>
-      <c r="B10" s="284"/>
-      <c r="C10" s="273" t="s">
-        <v>119</v>
-      </c>
-      <c r="D10" s="273"/>
-      <c r="E10" s="273"/>
-      <c r="F10" s="273"/>
-      <c r="G10" s="273"/>
-      <c r="H10" s="273"/>
-      <c r="I10" s="273"/>
-      <c r="J10" s="273"/>
-      <c r="K10" s="224"/>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" s="159">
-        <v>45658</v>
-      </c>
-      <c r="B11" s="160" t="s">
-        <v>120</v>
-      </c>
-      <c r="C11" s="182">
-        <f>C8</f>
-        <v>62500</v>
-      </c>
-      <c r="D11" s="182">
-        <f>D8</f>
-        <v>125000</v>
-      </c>
-      <c r="E11" s="182">
-        <f t="shared" ref="E11:H11" si="2">E8</f>
-        <v>208333.33333333334</v>
-      </c>
-      <c r="F11" s="182">
-        <f t="shared" si="2"/>
-        <v>83333.333333333328</v>
-      </c>
-      <c r="G11" s="182">
-        <f t="shared" si="2"/>
-        <v>291666.66666666669</v>
-      </c>
-      <c r="H11" s="182">
-        <f t="shared" si="2"/>
-        <v>75000</v>
-      </c>
-      <c r="I11" s="161"/>
-      <c r="J11" s="162"/>
-      <c r="K11" s="225">
-        <f>SUM(C11:J11)</f>
-        <v>845833.33333333337</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" s="163"/>
-      <c r="B12" s="164" t="s">
-        <v>121</v>
-      </c>
-      <c r="C12" s="114">
-        <v>500</v>
-      </c>
-      <c r="D12" s="114">
-        <v>300</v>
-      </c>
-      <c r="E12" s="114"/>
-      <c r="F12" s="114"/>
-      <c r="G12" s="114"/>
-      <c r="H12" s="114"/>
-      <c r="I12" s="114"/>
-      <c r="J12" s="165"/>
-      <c r="K12" s="226">
-        <f t="shared" ref="K12:K34" si="3">SUM(C12:J12)</f>
-        <v>800</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" s="159">
-        <v>45689</v>
-      </c>
-      <c r="B13" s="160" t="s">
-        <v>120</v>
-      </c>
-      <c r="C13" s="182">
-        <f>C8</f>
-        <v>62500</v>
-      </c>
-      <c r="D13" s="182">
-        <f>D8</f>
-        <v>125000</v>
-      </c>
-      <c r="E13" s="182">
-        <f t="shared" ref="E13:H13" si="4">E8</f>
-        <v>208333.33333333334</v>
-      </c>
-      <c r="F13" s="182">
-        <f t="shared" si="4"/>
-        <v>83333.333333333328</v>
-      </c>
-      <c r="G13" s="182">
-        <f t="shared" si="4"/>
-        <v>291666.66666666669</v>
-      </c>
-      <c r="H13" s="182">
-        <f t="shared" si="4"/>
-        <v>75000</v>
-      </c>
-      <c r="I13" s="161"/>
-      <c r="J13" s="162"/>
-      <c r="K13" s="225">
-        <f t="shared" si="3"/>
-        <v>845833.33333333337</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A14" s="163"/>
-      <c r="B14" s="164" t="s">
-        <v>121</v>
-      </c>
-      <c r="C14" s="114">
-        <v>0</v>
-      </c>
-      <c r="D14" s="114">
-        <v>300</v>
-      </c>
-      <c r="E14" s="114"/>
-      <c r="F14" s="114"/>
-      <c r="G14" s="114"/>
-      <c r="H14" s="114"/>
-      <c r="I14" s="114"/>
-      <c r="J14" s="165"/>
-      <c r="K14" s="226">
-        <f t="shared" si="3"/>
-        <v>300</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="159">
-        <v>45717</v>
-      </c>
-      <c r="B15" s="160" t="s">
-        <v>120</v>
-      </c>
-      <c r="C15" s="182">
-        <f>C13</f>
-        <v>62500</v>
-      </c>
-      <c r="D15" s="182">
-        <f t="shared" ref="D15:H15" si="5">D13</f>
-        <v>125000</v>
-      </c>
-      <c r="E15" s="182">
-        <f t="shared" si="5"/>
-        <v>208333.33333333334</v>
-      </c>
-      <c r="F15" s="182">
-        <f t="shared" si="5"/>
-        <v>83333.333333333328</v>
-      </c>
-      <c r="G15" s="182">
-        <f t="shared" si="5"/>
-        <v>291666.66666666669</v>
-      </c>
-      <c r="H15" s="182">
-        <f t="shared" si="5"/>
-        <v>75000</v>
-      </c>
-      <c r="I15" s="161"/>
-      <c r="J15" s="162"/>
-      <c r="K15" s="225">
-        <f t="shared" si="3"/>
-        <v>845833.33333333337</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" s="163"/>
-      <c r="B16" s="164" t="s">
-        <v>121</v>
-      </c>
-      <c r="C16" s="114">
-        <v>5000</v>
-      </c>
-      <c r="D16" s="114">
-        <v>10000</v>
-      </c>
-      <c r="E16" s="114">
-        <v>15000</v>
-      </c>
-      <c r="F16" s="114"/>
-      <c r="G16" s="114"/>
-      <c r="H16" s="114"/>
-      <c r="I16" s="114"/>
-      <c r="J16" s="165"/>
-      <c r="K16" s="226">
-        <f t="shared" si="3"/>
-        <v>30000</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" s="159">
-        <v>45748</v>
-      </c>
-      <c r="B17" s="160" t="s">
-        <v>120</v>
-      </c>
-      <c r="C17" s="161"/>
-      <c r="D17" s="161"/>
-      <c r="E17" s="161"/>
-      <c r="F17" s="161"/>
-      <c r="G17" s="161"/>
-      <c r="H17" s="161"/>
-      <c r="I17" s="161"/>
-      <c r="J17" s="162"/>
-      <c r="K17" s="225">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" s="163"/>
-      <c r="B18" s="164" t="s">
-        <v>121</v>
-      </c>
-      <c r="C18" s="114"/>
-      <c r="D18" s="114"/>
-      <c r="E18" s="114"/>
-      <c r="F18" s="114"/>
-      <c r="G18" s="114"/>
-      <c r="H18" s="114"/>
-      <c r="I18" s="114"/>
-      <c r="J18" s="165"/>
-      <c r="K18" s="226">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" s="159">
-        <v>45778</v>
-      </c>
-      <c r="B19" s="160" t="s">
-        <v>120</v>
-      </c>
-      <c r="C19" s="161"/>
-      <c r="D19" s="161"/>
-      <c r="E19" s="161"/>
-      <c r="F19" s="161"/>
-      <c r="G19" s="161"/>
-      <c r="H19" s="161"/>
-      <c r="I19" s="161"/>
-      <c r="J19" s="162"/>
-      <c r="K19" s="225">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" s="163"/>
-      <c r="B20" s="164" t="s">
-        <v>121</v>
-      </c>
-      <c r="C20" s="114"/>
-      <c r="D20" s="114"/>
-      <c r="E20" s="114"/>
-      <c r="F20" s="114"/>
-      <c r="G20" s="114"/>
-      <c r="H20" s="114"/>
-      <c r="I20" s="114"/>
-      <c r="J20" s="165"/>
-      <c r="K20" s="226">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" s="159">
-        <v>45809</v>
-      </c>
-      <c r="B21" s="160" t="s">
-        <v>120</v>
-      </c>
-      <c r="C21" s="161"/>
-      <c r="D21" s="161"/>
-      <c r="E21" s="161"/>
-      <c r="F21" s="161"/>
-      <c r="G21" s="161"/>
-      <c r="H21" s="161"/>
-      <c r="I21" s="161"/>
-      <c r="J21" s="162"/>
-      <c r="K21" s="225">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="163"/>
-      <c r="B22" s="164" t="s">
-        <v>121</v>
-      </c>
-      <c r="C22" s="114"/>
-      <c r="D22" s="114"/>
-      <c r="E22" s="114"/>
-      <c r="F22" s="114"/>
-      <c r="G22" s="114"/>
-      <c r="H22" s="114"/>
-      <c r="I22" s="114"/>
-      <c r="J22" s="165"/>
-      <c r="K22" s="226">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A23" s="159">
-        <v>45839</v>
-      </c>
-      <c r="B23" s="160" t="s">
-        <v>120</v>
-      </c>
-      <c r="C23" s="161"/>
-      <c r="D23" s="161"/>
-      <c r="E23" s="161"/>
-      <c r="F23" s="161"/>
-      <c r="G23" s="161"/>
-      <c r="H23" s="161"/>
-      <c r="I23" s="161"/>
-      <c r="J23" s="162"/>
-      <c r="K23" s="225">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A24" s="163"/>
-      <c r="B24" s="164" t="s">
-        <v>121</v>
-      </c>
-      <c r="C24" s="114"/>
-      <c r="D24" s="114"/>
-      <c r="E24" s="114"/>
-      <c r="F24" s="114"/>
-      <c r="G24" s="114"/>
-      <c r="H24" s="114"/>
-      <c r="I24" s="114"/>
-      <c r="J24" s="165"/>
-      <c r="K24" s="226">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A25" s="159">
-        <v>45870</v>
-      </c>
-      <c r="B25" s="160" t="s">
-        <v>120</v>
-      </c>
-      <c r="C25" s="161"/>
-      <c r="D25" s="161"/>
-      <c r="E25" s="161"/>
-      <c r="F25" s="161"/>
-      <c r="G25" s="161"/>
-      <c r="H25" s="161"/>
-      <c r="I25" s="161"/>
-      <c r="J25" s="162"/>
-      <c r="K25" s="225">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A26" s="163"/>
-      <c r="B26" s="164" t="s">
-        <v>121</v>
-      </c>
-      <c r="C26" s="114"/>
-      <c r="D26" s="114"/>
-      <c r="E26" s="114"/>
-      <c r="F26" s="114"/>
-      <c r="G26" s="114"/>
-      <c r="H26" s="114"/>
-      <c r="I26" s="114"/>
-      <c r="J26" s="165"/>
-      <c r="K26" s="226">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" s="159">
-        <v>45901</v>
-      </c>
-      <c r="B27" s="160" t="s">
-        <v>120</v>
-      </c>
-      <c r="C27" s="161"/>
-      <c r="D27" s="161"/>
-      <c r="E27" s="161"/>
-      <c r="F27" s="161"/>
-      <c r="G27" s="161"/>
-      <c r="H27" s="161"/>
-      <c r="I27" s="161"/>
-      <c r="J27" s="162"/>
-      <c r="K27" s="225">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" s="163"/>
-      <c r="B28" s="164" t="s">
-        <v>121</v>
-      </c>
-      <c r="C28" s="114"/>
-      <c r="D28" s="114"/>
-      <c r="E28" s="114"/>
-      <c r="F28" s="114"/>
-      <c r="G28" s="114"/>
-      <c r="H28" s="114"/>
-      <c r="I28" s="114"/>
-      <c r="J28" s="165"/>
-      <c r="K28" s="226">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="159">
-        <v>45931</v>
-      </c>
-      <c r="B29" s="160" t="s">
-        <v>120</v>
-      </c>
-      <c r="C29" s="161"/>
-      <c r="D29" s="161"/>
-      <c r="E29" s="161"/>
-      <c r="F29" s="161"/>
-      <c r="G29" s="161"/>
-      <c r="H29" s="161"/>
-      <c r="I29" s="161"/>
-      <c r="J29" s="162"/>
-      <c r="K29" s="225">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" s="163"/>
-      <c r="B30" s="164" t="s">
-        <v>121</v>
-      </c>
-      <c r="C30" s="114"/>
-      <c r="D30" s="114"/>
-      <c r="E30" s="114"/>
-      <c r="F30" s="114"/>
-      <c r="G30" s="114"/>
-      <c r="H30" s="114"/>
-      <c r="I30" s="114"/>
-      <c r="J30" s="165"/>
-      <c r="K30" s="226">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" s="159">
-        <v>45962</v>
-      </c>
-      <c r="B31" s="160" t="s">
-        <v>120</v>
-      </c>
-      <c r="C31" s="161"/>
-      <c r="D31" s="161"/>
-      <c r="E31" s="161"/>
-      <c r="F31" s="161"/>
-      <c r="G31" s="161"/>
-      <c r="H31" s="161"/>
-      <c r="I31" s="161"/>
-      <c r="J31" s="162"/>
-      <c r="K31" s="225">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" s="163"/>
-      <c r="B32" s="164" t="s">
-        <v>121</v>
-      </c>
-      <c r="C32" s="114"/>
-      <c r="D32" s="114"/>
-      <c r="E32" s="114"/>
-      <c r="F32" s="114"/>
-      <c r="G32" s="114"/>
-      <c r="H32" s="114"/>
-      <c r="I32" s="114"/>
-      <c r="J32" s="165"/>
-      <c r="K32" s="226">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" s="159">
-        <v>45992</v>
-      </c>
-      <c r="B33" s="160" t="s">
-        <v>120</v>
-      </c>
-      <c r="C33" s="161"/>
-      <c r="D33" s="161"/>
-      <c r="E33" s="161"/>
-      <c r="F33" s="161"/>
-      <c r="G33" s="161"/>
-      <c r="H33" s="161"/>
-      <c r="I33" s="161"/>
-      <c r="J33" s="162"/>
-      <c r="K33" s="225">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="183"/>
-      <c r="B34" s="184" t="s">
-        <v>121</v>
-      </c>
-      <c r="C34" s="104"/>
-      <c r="D34" s="104"/>
-      <c r="E34" s="104"/>
-      <c r="F34" s="104"/>
-      <c r="G34" s="104"/>
-      <c r="H34" s="104"/>
-      <c r="I34" s="104"/>
-      <c r="J34" s="185"/>
-      <c r="K34" s="228">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="186" t="s">
-        <v>122</v>
-      </c>
-      <c r="B35" s="187">
-        <f>SUM(C35:J35)</f>
-        <v>2506400</v>
-      </c>
-      <c r="C35" s="188">
-        <f>SUMIF($B11:$B34,$B11,C11:C34)-SUMIF($B11:$B34,$B12,C11:C34)</f>
-        <v>182000</v>
-      </c>
-      <c r="D35" s="188">
-        <f t="shared" ref="D35:J35" si="6">SUMIF($B11:$B34,$B11,D11:D34)-SUMIF($B11:$B34,$B12,D11:D34)</f>
-        <v>364400</v>
-      </c>
-      <c r="E35" s="188">
-        <f t="shared" si="6"/>
-        <v>610000</v>
-      </c>
-      <c r="F35" s="188">
-        <f t="shared" si="6"/>
-        <v>250000</v>
-      </c>
-      <c r="G35" s="188">
-        <f t="shared" si="6"/>
-        <v>875000</v>
-      </c>
-      <c r="H35" s="188">
-        <f t="shared" si="6"/>
-        <v>225000</v>
-      </c>
-      <c r="I35" s="188">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="J35" s="189">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="K35" s="227">
-        <f>SUM(K11:K34)</f>
-        <v>2568600</v>
-      </c>
+    <row r="10" spans="1:11" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="227"/>
+      <c r="B10" s="227"/>
+      <c r="C10" s="227"/>
+      <c r="D10" s="227"/>
+      <c r="E10" s="227"/>
+      <c r="F10" s="227"/>
+      <c r="G10" s="227"/>
+      <c r="H10" s="227"/>
+      <c r="I10" s="227"/>
+      <c r="J10" s="227"/>
+      <c r="K10" s="227"/>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="C10:J10"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A5:B5"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C5:K5">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>C$4</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThanOrEqual">
+      <formula>C$4</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0B4A6CE-E8DF-406D-9A73-D150B02B2C77}">
+  <sheetPr>
+    <tabColor rgb="FFFF00FF"/>
+  </sheetPr>
+  <dimension ref="A1:K28"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M10" sqref="M10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="14.21875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="17" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" s="10" customFormat="1" ht="20.399999999999999" x14ac:dyDescent="0.35">
+      <c r="A1" s="292" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="292"/>
+      <c r="C1" s="292"/>
+      <c r="D1" s="292"/>
+      <c r="E1" s="292"/>
+      <c r="F1" s="292"/>
+      <c r="G1" s="292"/>
+      <c r="H1" s="292"/>
+      <c r="I1" s="292"/>
+      <c r="J1" s="292"/>
+      <c r="K1" s="292"/>
+    </row>
+    <row r="2" spans="1:11" s="10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A2" s="228" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="228" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="290" t="s">
+        <v>157</v>
+      </c>
+      <c r="D2" s="290"/>
+      <c r="E2" s="290"/>
+      <c r="F2" s="290"/>
+      <c r="G2" s="290"/>
+      <c r="H2" s="290"/>
+      <c r="I2" s="290"/>
+      <c r="J2" s="290"/>
+      <c r="K2" s="228" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" s="10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A3" s="159">
+        <v>45658</v>
+      </c>
+      <c r="B3" s="160" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="232">
+        <f>Subcontractors!C9</f>
+        <v>62500</v>
+      </c>
+      <c r="D3" s="232">
+        <f>Subcontractors!D9</f>
+        <v>125000</v>
+      </c>
+      <c r="E3" s="232">
+        <f>Subcontractors!E9</f>
+        <v>208333.33333333334</v>
+      </c>
+      <c r="F3" s="232">
+        <f>Subcontractors!F9</f>
+        <v>83333.333333333328</v>
+      </c>
+      <c r="G3" s="232">
+        <f>Subcontractors!G9</f>
+        <v>291666.66666666669</v>
+      </c>
+      <c r="H3" s="232">
+        <f>Subcontractors!H9</f>
+        <v>75000</v>
+      </c>
+      <c r="I3" s="232">
+        <f>Subcontractors!I9</f>
+        <v>0</v>
+      </c>
+      <c r="J3" s="232">
+        <f>Subcontractors!J9</f>
+        <v>0</v>
+      </c>
+      <c r="K3" s="229">
+        <f>SUM(C3:J3)</f>
+        <v>845833.33333333337</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" s="10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A4" s="161"/>
+      <c r="B4" s="162" t="s">
+        <v>119</v>
+      </c>
+      <c r="C4" s="76">
+        <v>-500</v>
+      </c>
+      <c r="D4" s="76">
+        <v>-300</v>
+      </c>
+      <c r="E4" s="76"/>
+      <c r="F4" s="76"/>
+      <c r="G4" s="76"/>
+      <c r="H4" s="76"/>
+      <c r="I4" s="76"/>
+      <c r="J4" s="233"/>
+      <c r="K4" s="230">
+        <f t="shared" ref="K4:K26" si="0">SUM(C4:J4)</f>
+        <v>-800</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" s="10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A5" s="159">
+        <v>45689</v>
+      </c>
+      <c r="B5" s="160" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" s="232">
+        <f>C3</f>
+        <v>62500</v>
+      </c>
+      <c r="D5" s="232">
+        <f t="shared" ref="D5:J5" si="1">D3</f>
+        <v>125000</v>
+      </c>
+      <c r="E5" s="232">
+        <f t="shared" si="1"/>
+        <v>208333.33333333334</v>
+      </c>
+      <c r="F5" s="232">
+        <f t="shared" si="1"/>
+        <v>83333.333333333328</v>
+      </c>
+      <c r="G5" s="232">
+        <f t="shared" si="1"/>
+        <v>291666.66666666669</v>
+      </c>
+      <c r="H5" s="232">
+        <f t="shared" si="1"/>
+        <v>75000</v>
+      </c>
+      <c r="I5" s="232">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J5" s="232">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="K5" s="229">
+        <f t="shared" si="0"/>
+        <v>845833.33333333337</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" s="10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A6" s="161"/>
+      <c r="B6" s="162" t="s">
+        <v>119</v>
+      </c>
+      <c r="C6" s="76">
+        <v>0</v>
+      </c>
+      <c r="D6" s="76">
+        <v>-300</v>
+      </c>
+      <c r="E6" s="76"/>
+      <c r="F6" s="76"/>
+      <c r="G6" s="76"/>
+      <c r="H6" s="76"/>
+      <c r="I6" s="76"/>
+      <c r="J6" s="233"/>
+      <c r="K6" s="230">
+        <f t="shared" si="0"/>
+        <v>-300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A7" s="159">
+        <v>45717</v>
+      </c>
+      <c r="B7" s="160" t="s">
+        <v>118</v>
+      </c>
+      <c r="C7" s="232">
+        <f>C5</f>
+        <v>62500</v>
+      </c>
+      <c r="D7" s="232">
+        <f t="shared" ref="D7:H7" si="2">D5</f>
+        <v>125000</v>
+      </c>
+      <c r="E7" s="232">
+        <f t="shared" si="2"/>
+        <v>208333.33333333334</v>
+      </c>
+      <c r="F7" s="232">
+        <f t="shared" si="2"/>
+        <v>83333.333333333328</v>
+      </c>
+      <c r="G7" s="232">
+        <f t="shared" si="2"/>
+        <v>291666.66666666669</v>
+      </c>
+      <c r="H7" s="232">
+        <f t="shared" si="2"/>
+        <v>75000</v>
+      </c>
+      <c r="I7" s="232"/>
+      <c r="J7" s="234"/>
+      <c r="K7" s="229">
+        <f t="shared" si="0"/>
+        <v>845833.33333333337</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A8" s="161"/>
+      <c r="B8" s="162" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="76">
+        <v>-5000</v>
+      </c>
+      <c r="D8" s="76">
+        <v>-10000</v>
+      </c>
+      <c r="E8" s="76">
+        <v>-15000</v>
+      </c>
+      <c r="F8" s="76"/>
+      <c r="G8" s="76"/>
+      <c r="H8" s="76"/>
+      <c r="I8" s="76"/>
+      <c r="J8" s="233"/>
+      <c r="K8" s="230">
+        <f t="shared" si="0"/>
+        <v>-30000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A9" s="159">
+        <v>45748</v>
+      </c>
+      <c r="B9" s="160" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="232"/>
+      <c r="D9" s="232"/>
+      <c r="E9" s="232"/>
+      <c r="F9" s="232"/>
+      <c r="G9" s="232"/>
+      <c r="H9" s="232"/>
+      <c r="I9" s="232"/>
+      <c r="J9" s="234"/>
+      <c r="K9" s="229">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A10" s="161"/>
+      <c r="B10" s="162" t="s">
+        <v>119</v>
+      </c>
+      <c r="C10" s="76"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="76"/>
+      <c r="G10" s="76"/>
+      <c r="H10" s="76"/>
+      <c r="I10" s="76"/>
+      <c r="J10" s="233"/>
+      <c r="K10" s="230">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A11" s="159">
+        <v>45778</v>
+      </c>
+      <c r="B11" s="160" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="232"/>
+      <c r="D11" s="232"/>
+      <c r="E11" s="232"/>
+      <c r="F11" s="232"/>
+      <c r="G11" s="232"/>
+      <c r="H11" s="232"/>
+      <c r="I11" s="232"/>
+      <c r="J11" s="234"/>
+      <c r="K11" s="229">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A12" s="161"/>
+      <c r="B12" s="162" t="s">
+        <v>119</v>
+      </c>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="76"/>
+      <c r="G12" s="76"/>
+      <c r="H12" s="76"/>
+      <c r="I12" s="76"/>
+      <c r="J12" s="233"/>
+      <c r="K12" s="230">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A13" s="159">
+        <v>45809</v>
+      </c>
+      <c r="B13" s="160" t="s">
+        <v>118</v>
+      </c>
+      <c r="C13" s="232"/>
+      <c r="D13" s="232"/>
+      <c r="E13" s="232"/>
+      <c r="F13" s="232"/>
+      <c r="G13" s="232"/>
+      <c r="H13" s="232"/>
+      <c r="I13" s="232"/>
+      <c r="J13" s="234"/>
+      <c r="K13" s="229">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A14" s="161"/>
+      <c r="B14" s="162" t="s">
+        <v>119</v>
+      </c>
+      <c r="C14" s="76"/>
+      <c r="D14" s="76"/>
+      <c r="E14" s="76"/>
+      <c r="F14" s="76"/>
+      <c r="G14" s="76"/>
+      <c r="H14" s="76"/>
+      <c r="I14" s="76"/>
+      <c r="J14" s="233"/>
+      <c r="K14" s="230">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" s="10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A15" s="159">
+        <v>45839</v>
+      </c>
+      <c r="B15" s="160" t="s">
+        <v>118</v>
+      </c>
+      <c r="C15" s="232"/>
+      <c r="D15" s="232"/>
+      <c r="E15" s="232"/>
+      <c r="F15" s="232"/>
+      <c r="G15" s="232"/>
+      <c r="H15" s="232"/>
+      <c r="I15" s="232"/>
+      <c r="J15" s="234"/>
+      <c r="K15" s="229">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" s="10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A16" s="161"/>
+      <c r="B16" s="162" t="s">
+        <v>119</v>
+      </c>
+      <c r="C16" s="76"/>
+      <c r="D16" s="76"/>
+      <c r="E16" s="76"/>
+      <c r="F16" s="76"/>
+      <c r="G16" s="76"/>
+      <c r="H16" s="76"/>
+      <c r="I16" s="76"/>
+      <c r="J16" s="233"/>
+      <c r="K16" s="230">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A17" s="159">
+        <v>45870</v>
+      </c>
+      <c r="B17" s="160" t="s">
+        <v>118</v>
+      </c>
+      <c r="C17" s="232"/>
+      <c r="D17" s="232"/>
+      <c r="E17" s="232"/>
+      <c r="F17" s="232"/>
+      <c r="G17" s="232"/>
+      <c r="H17" s="232"/>
+      <c r="I17" s="232"/>
+      <c r="J17" s="234"/>
+      <c r="K17" s="229">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" s="10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A18" s="161"/>
+      <c r="B18" s="162" t="s">
+        <v>119</v>
+      </c>
+      <c r="C18" s="76"/>
+      <c r="D18" s="76"/>
+      <c r="E18" s="76"/>
+      <c r="F18" s="76"/>
+      <c r="G18" s="76"/>
+      <c r="H18" s="76"/>
+      <c r="I18" s="76"/>
+      <c r="J18" s="233"/>
+      <c r="K18" s="230">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A19" s="159">
+        <v>45901</v>
+      </c>
+      <c r="B19" s="160" t="s">
+        <v>118</v>
+      </c>
+      <c r="C19" s="232"/>
+      <c r="D19" s="232"/>
+      <c r="E19" s="232"/>
+      <c r="F19" s="232"/>
+      <c r="G19" s="232"/>
+      <c r="H19" s="232"/>
+      <c r="I19" s="232"/>
+      <c r="J19" s="234"/>
+      <c r="K19" s="229">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A20" s="161"/>
+      <c r="B20" s="162" t="s">
+        <v>119</v>
+      </c>
+      <c r="C20" s="76"/>
+      <c r="D20" s="76"/>
+      <c r="E20" s="76"/>
+      <c r="F20" s="76"/>
+      <c r="G20" s="76"/>
+      <c r="H20" s="76"/>
+      <c r="I20" s="76"/>
+      <c r="J20" s="233"/>
+      <c r="K20" s="230">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" s="10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A21" s="159">
+        <v>45931</v>
+      </c>
+      <c r="B21" s="160" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" s="232"/>
+      <c r="D21" s="232"/>
+      <c r="E21" s="232"/>
+      <c r="F21" s="232"/>
+      <c r="G21" s="232"/>
+      <c r="H21" s="232"/>
+      <c r="I21" s="232"/>
+      <c r="J21" s="234"/>
+      <c r="K21" s="229">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" s="10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A22" s="161"/>
+      <c r="B22" s="162" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="76"/>
+      <c r="D22" s="76"/>
+      <c r="E22" s="76"/>
+      <c r="F22" s="76"/>
+      <c r="G22" s="76"/>
+      <c r="H22" s="76"/>
+      <c r="I22" s="76"/>
+      <c r="J22" s="233"/>
+      <c r="K22" s="230">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" s="10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A23" s="159">
+        <v>45962</v>
+      </c>
+      <c r="B23" s="160" t="s">
+        <v>118</v>
+      </c>
+      <c r="C23" s="232"/>
+      <c r="D23" s="232"/>
+      <c r="E23" s="232"/>
+      <c r="F23" s="232"/>
+      <c r="G23" s="232"/>
+      <c r="H23" s="232"/>
+      <c r="I23" s="232"/>
+      <c r="J23" s="234"/>
+      <c r="K23" s="229">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" s="10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A24" s="161"/>
+      <c r="B24" s="162" t="s">
+        <v>119</v>
+      </c>
+      <c r="C24" s="76"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="76"/>
+      <c r="F24" s="76"/>
+      <c r="G24" s="76"/>
+      <c r="H24" s="76"/>
+      <c r="I24" s="76"/>
+      <c r="J24" s="233"/>
+      <c r="K24" s="230">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" s="10" customFormat="1" ht="13.8" x14ac:dyDescent="0.25">
+      <c r="A25" s="159">
+        <v>45992</v>
+      </c>
+      <c r="B25" s="160" t="s">
+        <v>118</v>
+      </c>
+      <c r="C25" s="232"/>
+      <c r="D25" s="232"/>
+      <c r="E25" s="232"/>
+      <c r="F25" s="232"/>
+      <c r="G25" s="232"/>
+      <c r="H25" s="232"/>
+      <c r="I25" s="232"/>
+      <c r="J25" s="234"/>
+      <c r="K25" s="229">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" s="10" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="174"/>
+      <c r="B26" s="175" t="s">
+        <v>119</v>
+      </c>
+      <c r="C26" s="235"/>
+      <c r="D26" s="235"/>
+      <c r="E26" s="235"/>
+      <c r="F26" s="235"/>
+      <c r="G26" s="235"/>
+      <c r="H26" s="235"/>
+      <c r="I26" s="235"/>
+      <c r="J26" s="236"/>
+      <c r="K26" s="231">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" s="10" customFormat="1" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="176" t="s">
+        <v>120</v>
+      </c>
+      <c r="B27" s="177">
+        <f>SUM(C27:J27)</f>
+        <v>2506400</v>
+      </c>
+      <c r="C27" s="178">
+        <f>SUM(C3:C26)</f>
+        <v>182000</v>
+      </c>
+      <c r="D27" s="178">
+        <f t="shared" ref="D27:J27" si="3">SUM(D3:D26)</f>
+        <v>364400</v>
+      </c>
+      <c r="E27" s="178">
+        <f t="shared" si="3"/>
+        <v>610000</v>
+      </c>
+      <c r="F27" s="178">
+        <f t="shared" si="3"/>
+        <v>250000</v>
+      </c>
+      <c r="G27" s="178">
+        <f t="shared" si="3"/>
+        <v>875000</v>
+      </c>
+      <c r="H27" s="178">
+        <f t="shared" si="3"/>
+        <v>225000</v>
+      </c>
+      <c r="I27" s="178">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J27" s="178">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="K27" s="211">
+        <f>SUM(K3:K26)</f>
+        <v>2506400</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="291" t="s">
+        <v>117</v>
+      </c>
+      <c r="B28" s="291"/>
+      <c r="C28" s="291"/>
+      <c r="D28" s="291"/>
+      <c r="E28" s="291"/>
+      <c r="F28" s="291"/>
+      <c r="G28" s="291"/>
+      <c r="H28" s="291"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="A28:H28"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4491,7 +4790,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4504,31 +4803,31 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="33.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="238" t="s">
+      <c r="A1" s="243" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="235" t="s">
+      <c r="B1" s="240" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="236"/>
-      <c r="D1" s="237"/>
-      <c r="E1" s="235" t="s">
+      <c r="C1" s="241"/>
+      <c r="D1" s="242"/>
+      <c r="E1" s="240" t="s">
         <v>19</v>
       </c>
-      <c r="F1" s="236"/>
-      <c r="G1" s="237"/>
-      <c r="H1" s="240" t="s">
+      <c r="F1" s="241"/>
+      <c r="G1" s="242"/>
+      <c r="H1" s="245" t="s">
         <v>20</v>
       </c>
-      <c r="I1" s="241"/>
-      <c r="J1" s="235" t="s">
+      <c r="I1" s="246"/>
+      <c r="J1" s="240" t="s">
         <v>21</v>
       </c>
-      <c r="K1" s="236"/>
-      <c r="L1" s="237"/>
+      <c r="K1" s="241"/>
+      <c r="L1" s="242"/>
     </row>
     <row r="2" spans="1:12" s="15" customFormat="1" ht="41.4" x14ac:dyDescent="0.25">
-      <c r="A2" s="239"/>
+      <c r="A2" s="244"/>
       <c r="B2" s="63" t="s">
         <v>10</v>
       </c>
@@ -4567,7 +4866,7 @@
       <c r="A3" s="16">
         <v>45688</v>
       </c>
-      <c r="B3" s="202">
+      <c r="B3" s="191">
         <f>('Project Overview'!$D$7/DATEDIF('Project Overview'!$D$5, 'Project Overview'!$D$6, "M")) *80%</f>
         <v>1619512.1951219514</v>
       </c>
@@ -4579,7 +4878,7 @@
         <f t="shared" ref="D3:D5" si="0">IF(C3&gt;0,C3-B3,0)</f>
         <v>-141478.86178861791</v>
       </c>
-      <c r="E3" s="202">
+      <c r="E3" s="191">
         <f>Billing!E2</f>
         <v>1850000</v>
       </c>
@@ -4612,7 +4911,7 @@
       <c r="A4" s="16">
         <v>45716</v>
       </c>
-      <c r="B4" s="202">
+      <c r="B4" s="191">
         <f>('Project Overview'!$D$7/DATEDIF('Project Overview'!$D$5, 'Project Overview'!$D$6, "M")) *80%</f>
         <v>1619512.1951219514</v>
       </c>
@@ -4624,7 +4923,7 @@
         <f t="shared" si="0"/>
         <v>-490618.86178861791</v>
       </c>
-      <c r="E4" s="202">
+      <c r="E4" s="191">
         <f>Billing!E3</f>
         <v>1630000</v>
       </c>
@@ -4657,7 +4956,7 @@
       <c r="A5" s="16">
         <v>45747</v>
       </c>
-      <c r="B5" s="202">
+      <c r="B5" s="191">
         <f>('Project Overview'!$D$7/DATEDIF('Project Overview'!$D$5, 'Project Overview'!$D$6, "M")) *80%</f>
         <v>1619512.1951219514</v>
       </c>
@@ -4669,7 +4968,7 @@
         <f t="shared" si="0"/>
         <v>-226247.86178861791</v>
       </c>
-      <c r="E5" s="202">
+      <c r="E5" s="191">
         <f>Billing!E4</f>
         <v>1800000</v>
       </c>
@@ -5054,7 +5353,7 @@
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A17" s="203" t="s">
+      <c r="A17" s="192" t="s">
         <v>50</v>
       </c>
       <c r="B17" s="10" t="s">
@@ -5082,8 +5381,8 @@
   </sheetPr>
   <dimension ref="A1:O12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N8" sqref="N8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="27.6" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -5147,7 +5446,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
@@ -5168,7 +5467,7 @@
         <v>1.1000000000000001</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C3" s="25">
         <v>350000</v>
@@ -5198,7 +5497,7 @@
         <v>1.2</v>
       </c>
       <c r="B4" s="22" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C4" s="27">
         <v>80000</v>
@@ -5287,7 +5586,7 @@
         <v>2</v>
       </c>
       <c r="B6" s="24" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C6" s="29">
         <v>100000</v>
@@ -5317,7 +5616,7 @@
         <v>3</v>
       </c>
       <c r="B7" s="18" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C7" s="25">
         <v>50000</v>
@@ -5347,54 +5646,54 @@
         <v>4</v>
       </c>
       <c r="B8" s="18" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C8" s="25">
-        <f>Subcontractors!K11-Subcontractors!K12</f>
+        <f>'Subcontractor Monthly Billing'!K3+'Subcontractor Monthly Billing'!K4</f>
         <v>845033.33333333337</v>
       </c>
       <c r="D8" s="25">
-        <f>Subcontractors!K13-Subcontractors!K14</f>
+        <f>SUM('Subcontractor Monthly Billing'!K5:K6)</f>
         <v>845533.33333333337</v>
       </c>
       <c r="E8" s="25">
-        <f>Subcontractors!K15-Subcontractors!K16</f>
+        <f>SUM('Subcontractor Monthly Billing'!K7:K8)</f>
         <v>815833.33333333337</v>
       </c>
       <c r="F8" s="25">
-        <f>Subcontractors!K17-Subcontractors!K18</f>
+        <f>SUM('Subcontractor Monthly Billing'!K9:K10)</f>
         <v>0</v>
       </c>
       <c r="G8" s="25">
-        <f>Subcontractors!K19-Subcontractors!K20</f>
+        <f>SUM('Subcontractor Monthly Billing'!K11:K12)</f>
         <v>0</v>
       </c>
       <c r="H8" s="25">
-        <f>Subcontractors!K21-Subcontractors!K22</f>
+        <f>SUM('Subcontractor Monthly Billing'!K13:K14)</f>
         <v>0</v>
       </c>
       <c r="I8" s="25">
-        <f>Subcontractors!K23-Subcontractors!K24</f>
+        <f>SUM('Subcontractor Monthly Billing'!K15:K16)</f>
         <v>0</v>
       </c>
       <c r="J8" s="25">
-        <f>Subcontractors!K25-Subcontractors!K26</f>
+        <f>SUM('Subcontractor Monthly Billing'!K17:K18)</f>
         <v>0</v>
       </c>
       <c r="K8" s="25">
-        <f>Subcontractors!K27-Subcontractors!K28</f>
+        <f>SUM('Subcontractor Monthly Billing'!K19:K20)</f>
         <v>0</v>
       </c>
       <c r="L8" s="25">
-        <f>Subcontractors!K29-Subcontractors!K30</f>
+        <f>SUM('Subcontractor Monthly Billing'!K21:K22)</f>
         <v>0</v>
       </c>
       <c r="M8" s="25">
-        <f>Subcontractors!K31-Subcontractors!K32</f>
+        <f>SUM('Subcontractor Monthly Billing'!K23:K24)</f>
         <v>0</v>
       </c>
       <c r="N8" s="25">
-        <f>Subcontractors!K33-Subcontractors!K34</f>
+        <f>SUM('Subcontractor Monthly Billing'!K25:K26)</f>
         <v>0</v>
       </c>
       <c r="O8" s="26">
@@ -5407,7 +5706,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C9" s="25">
         <v>3000</v>
@@ -5437,7 +5736,7 @@
         <v>6</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C10" s="25">
         <v>50000</v>
@@ -5467,7 +5766,7 @@
         <v>7</v>
       </c>
       <c r="B11" s="23" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C11" s="27">
         <v>0</v>
@@ -5570,36 +5869,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="31.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="215" t="s">
+      <c r="A1" s="204" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="216" t="s">
+      <c r="B1" s="205" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="217" t="s">
+      <c r="C1" s="206" t="s">
         <v>32</v>
       </c>
-      <c r="D1" s="217" t="s">
+      <c r="D1" s="206" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="217" t="s">
+      <c r="E1" s="206" t="s">
         <v>33</v>
       </c>
-      <c r="F1" s="217" t="s">
+      <c r="F1" s="206" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="218" t="s">
+      <c r="G1" s="207" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="212">
+      <c r="A2" s="201">
         <v>45688</v>
       </c>
-      <c r="B2" s="213">
+      <c r="B2" s="202">
         <v>0.85</v>
       </c>
-      <c r="C2" s="202">
+      <c r="C2" s="191">
         <f>'Project Overview'!$D$7/DATEDIF('Project Overview'!$D$5, 'Project Overview'!$D$6, "M")</f>
         <v>2024390.243902439</v>
       </c>
@@ -5617,13 +5916,13 @@
       <c r="F2" s="35">
         <v>5000</v>
       </c>
-      <c r="G2" s="214">
+      <c r="G2" s="203">
         <f>IF(C2&lt;&gt;"",C2-E2-F2,0)</f>
         <v>1999146.3414634147</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="212">
+      <c r="A3" s="201">
         <v>45716</v>
       </c>
       <c r="B3" s="71">
@@ -5646,13 +5945,13 @@
       <c r="F3" s="37">
         <v>10000</v>
       </c>
-      <c r="G3" s="214">
+      <c r="G3" s="203">
         <f t="shared" ref="G3:G13" si="1">IF(C3&lt;&gt;"",C3-E3-F3,0)</f>
         <v>1714390.243902439</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="212">
+      <c r="A4" s="201">
         <v>45747</v>
       </c>
       <c r="B4" s="71">
@@ -5675,13 +5974,13 @@
       <c r="F4" s="37">
         <v>3000</v>
       </c>
-      <c r="G4" s="214">
+      <c r="G4" s="203">
         <f t="shared" si="1"/>
         <v>1844414.6341463414</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="212">
+      <c r="A5" s="201">
         <v>45777</v>
       </c>
       <c r="B5" s="73"/>
@@ -5698,13 +5997,13 @@
         <v/>
       </c>
       <c r="F5" s="74"/>
-      <c r="G5" s="214">
+      <c r="G5" s="203">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="212">
+      <c r="A6" s="201">
         <v>45808</v>
       </c>
       <c r="B6" s="73"/>
@@ -5721,13 +6020,13 @@
         <v/>
       </c>
       <c r="F6" s="74"/>
-      <c r="G6" s="214">
+      <c r="G6" s="203">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="212">
+      <c r="A7" s="201">
         <v>45838</v>
       </c>
       <c r="B7" s="73"/>
@@ -5744,13 +6043,13 @@
         <v/>
       </c>
       <c r="F7" s="74"/>
-      <c r="G7" s="214">
+      <c r="G7" s="203">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="212">
+      <c r="A8" s="201">
         <v>45869</v>
       </c>
       <c r="B8" s="73"/>
@@ -5767,13 +6066,13 @@
         <v/>
       </c>
       <c r="F8" s="74"/>
-      <c r="G8" s="214">
+      <c r="G8" s="203">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="212">
+      <c r="A9" s="201">
         <v>45900</v>
       </c>
       <c r="B9" s="73"/>
@@ -5790,13 +6089,13 @@
         <v/>
       </c>
       <c r="F9" s="74"/>
-      <c r="G9" s="214">
+      <c r="G9" s="203">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="212">
+      <c r="A10" s="201">
         <v>45930</v>
       </c>
       <c r="B10" s="73"/>
@@ -5813,13 +6112,13 @@
         <v/>
       </c>
       <c r="F10" s="74"/>
-      <c r="G10" s="214">
+      <c r="G10" s="203">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="212">
+      <c r="A11" s="201">
         <v>45961</v>
       </c>
       <c r="B11" s="73"/>
@@ -5836,13 +6135,13 @@
         <v/>
       </c>
       <c r="F11" s="74"/>
-      <c r="G11" s="214">
+      <c r="G11" s="203">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="212">
+      <c r="A12" s="201">
         <v>45991</v>
       </c>
       <c r="B12" s="73"/>
@@ -5859,13 +6158,13 @@
         <v/>
       </c>
       <c r="F12" s="74"/>
-      <c r="G12" s="214">
+      <c r="G12" s="203">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="212">
+      <c r="A13" s="201">
         <v>46022</v>
       </c>
       <c r="B13" s="75"/>
@@ -5882,7 +6181,7 @@
         <v/>
       </c>
       <c r="F13" s="76"/>
-      <c r="G13" s="214">
+      <c r="G13" s="203">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
@@ -6261,94 +6560,94 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="245" t="s">
+      <c r="A1" s="250" t="s">
         <v>102</v>
       </c>
-      <c r="B1" s="247" t="s">
+      <c r="B1" s="252" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" s="256" t="s">
+        <v>146</v>
+      </c>
+      <c r="D1" s="258" t="s">
+        <v>150</v>
+      </c>
+      <c r="E1" s="254" t="s">
+        <v>122</v>
+      </c>
+      <c r="F1" s="247" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="251" t="s">
-        <v>148</v>
-      </c>
-      <c r="D1" s="253" t="s">
-        <v>152</v>
-      </c>
-      <c r="E1" s="249" t="s">
+      <c r="G1" s="248"/>
+      <c r="H1" s="248"/>
+      <c r="I1" s="248"/>
+      <c r="J1" s="248"/>
+      <c r="K1" s="248"/>
+      <c r="L1" s="248"/>
+      <c r="M1" s="248"/>
+      <c r="N1" s="248"/>
+      <c r="O1" s="248"/>
+      <c r="P1" s="248"/>
+      <c r="Q1" s="249"/>
+    </row>
+    <row r="2" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="251"/>
+      <c r="B2" s="253"/>
+      <c r="C2" s="257"/>
+      <c r="D2" s="259"/>
+      <c r="E2" s="255"/>
+      <c r="F2" s="179">
+        <v>45688</v>
+      </c>
+      <c r="G2" s="179">
+        <v>45716</v>
+      </c>
+      <c r="H2" s="179">
+        <v>45747</v>
+      </c>
+      <c r="I2" s="179">
+        <v>45777</v>
+      </c>
+      <c r="J2" s="179">
+        <v>45808</v>
+      </c>
+      <c r="K2" s="179">
+        <v>45838</v>
+      </c>
+      <c r="L2" s="179">
+        <v>45869</v>
+      </c>
+      <c r="M2" s="179">
+        <v>45900</v>
+      </c>
+      <c r="N2" s="179">
+        <v>45930</v>
+      </c>
+      <c r="O2" s="179">
+        <v>45961</v>
+      </c>
+      <c r="P2" s="179">
+        <v>45991</v>
+      </c>
+      <c r="Q2" s="179">
+        <v>46022</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="180">
+        <v>1</v>
+      </c>
+      <c r="B3" s="181" t="s">
         <v>124</v>
       </c>
-      <c r="F1" s="242" t="s">
-        <v>125</v>
-      </c>
-      <c r="G1" s="243"/>
-      <c r="H1" s="243"/>
-      <c r="I1" s="243"/>
-      <c r="J1" s="243"/>
-      <c r="K1" s="243"/>
-      <c r="L1" s="243"/>
-      <c r="M1" s="243"/>
-      <c r="N1" s="243"/>
-      <c r="O1" s="243"/>
-      <c r="P1" s="243"/>
-      <c r="Q1" s="244"/>
-    </row>
-    <row r="2" spans="1:17" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="246"/>
-      <c r="B2" s="248"/>
-      <c r="C2" s="252"/>
-      <c r="D2" s="254"/>
-      <c r="E2" s="250"/>
-      <c r="F2" s="190">
-        <v>45688</v>
-      </c>
-      <c r="G2" s="190">
-        <v>45716</v>
-      </c>
-      <c r="H2" s="190">
-        <v>45747</v>
-      </c>
-      <c r="I2" s="190">
-        <v>45777</v>
-      </c>
-      <c r="J2" s="190">
-        <v>45808</v>
-      </c>
-      <c r="K2" s="190">
-        <v>45838</v>
-      </c>
-      <c r="L2" s="190">
-        <v>45869</v>
-      </c>
-      <c r="M2" s="190">
-        <v>45900</v>
-      </c>
-      <c r="N2" s="190">
-        <v>45930</v>
-      </c>
-      <c r="O2" s="190">
-        <v>45961</v>
-      </c>
-      <c r="P2" s="190">
-        <v>45991</v>
-      </c>
-      <c r="Q2" s="190">
-        <v>46022</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="191">
+      <c r="C3" s="193"/>
+      <c r="D3" s="193">
         <v>1</v>
       </c>
-      <c r="B3" s="192" t="s">
-        <v>126</v>
-      </c>
-      <c r="C3" s="204"/>
-      <c r="D3" s="204">
+      <c r="E3" s="182">
         <v>1</v>
       </c>
-      <c r="E3" s="193">
-        <v>1</v>
-      </c>
-      <c r="F3" s="166">
+      <c r="F3" s="163">
         <v>1</v>
       </c>
       <c r="G3" s="95">
@@ -6368,22 +6667,22 @@
       <c r="Q3" s="96"/>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="194">
+      <c r="A4" s="183">
         <v>2</v>
       </c>
-      <c r="B4" s="195" t="s">
-        <v>127</v>
-      </c>
-      <c r="C4" s="205" t="s">
-        <v>126</v>
-      </c>
-      <c r="D4" s="205">
+      <c r="B4" s="184" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="194" t="s">
+        <v>124</v>
+      </c>
+      <c r="D4" s="194">
         <v>2</v>
       </c>
-      <c r="E4" s="196">
+      <c r="E4" s="185">
         <v>1</v>
       </c>
-      <c r="F4" s="169">
+      <c r="F4" s="164">
         <v>1</v>
       </c>
       <c r="G4" s="99">
@@ -6403,22 +6702,22 @@
       <c r="Q4" s="100"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" s="194">
+      <c r="A5" s="183">
         <v>3</v>
       </c>
-      <c r="B5" s="195" t="s">
-        <v>128</v>
-      </c>
-      <c r="C5" s="205" t="s">
+      <c r="B5" s="184" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="205">
+      <c r="C5" s="194" t="s">
+        <v>124</v>
+      </c>
+      <c r="D5" s="194">
         <v>2</v>
       </c>
-      <c r="E5" s="196">
+      <c r="E5" s="185">
         <v>1</v>
       </c>
-      <c r="F5" s="169">
+      <c r="F5" s="164">
         <v>1</v>
       </c>
       <c r="G5" s="99">
@@ -6438,22 +6737,22 @@
       <c r="Q5" s="100"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="194">
+      <c r="A6" s="183">
         <v>4</v>
       </c>
-      <c r="B6" s="195" t="s">
-        <v>129</v>
-      </c>
-      <c r="C6" s="205" t="s">
-        <v>126</v>
-      </c>
-      <c r="D6" s="205">
+      <c r="B6" s="184" t="s">
+        <v>127</v>
+      </c>
+      <c r="C6" s="194" t="s">
+        <v>124</v>
+      </c>
+      <c r="D6" s="194">
         <v>2</v>
       </c>
-      <c r="E6" s="196">
+      <c r="E6" s="185">
         <v>1</v>
       </c>
-      <c r="F6" s="169">
+      <c r="F6" s="164">
         <v>1</v>
       </c>
       <c r="G6" s="99">
@@ -6473,22 +6772,22 @@
       <c r="Q6" s="100"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="194">
+      <c r="A7" s="183">
         <v>5</v>
       </c>
-      <c r="B7" s="195" t="s">
-        <v>130</v>
-      </c>
-      <c r="C7" s="205" t="s">
-        <v>126</v>
-      </c>
-      <c r="D7" s="205">
+      <c r="B7" s="184" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" s="194" t="s">
+        <v>124</v>
+      </c>
+      <c r="D7" s="194">
         <v>2</v>
       </c>
-      <c r="E7" s="196">
+      <c r="E7" s="185">
         <v>1</v>
       </c>
-      <c r="F7" s="169">
+      <c r="F7" s="164">
         <v>1</v>
       </c>
       <c r="G7" s="99">
@@ -6508,22 +6807,22 @@
       <c r="Q7" s="100"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="194">
+      <c r="A8" s="183">
         <v>6</v>
       </c>
-      <c r="B8" s="195" t="s">
-        <v>147</v>
-      </c>
-      <c r="C8" s="205" t="s">
-        <v>128</v>
-      </c>
-      <c r="D8" s="205">
+      <c r="B8" s="184" t="s">
+        <v>145</v>
+      </c>
+      <c r="C8" s="194" t="s">
+        <v>126</v>
+      </c>
+      <c r="D8" s="194">
         <v>3</v>
       </c>
-      <c r="E8" s="196">
+      <c r="E8" s="185">
         <v>4</v>
       </c>
-      <c r="F8" s="169">
+      <c r="F8" s="164">
         <v>5</v>
       </c>
       <c r="G8" s="99">
@@ -6543,22 +6842,22 @@
       <c r="Q8" s="100"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9" s="194">
+      <c r="A9" s="183">
         <v>7</v>
       </c>
-      <c r="B9" s="195" t="s">
-        <v>149</v>
-      </c>
-      <c r="C9" s="205" t="s">
+      <c r="B9" s="184" t="s">
         <v>147</v>
       </c>
-      <c r="D9" s="205">
+      <c r="C9" s="194" t="s">
+        <v>145</v>
+      </c>
+      <c r="D9" s="194">
         <v>4</v>
       </c>
-      <c r="E9" s="196">
+      <c r="E9" s="185">
         <v>1</v>
       </c>
-      <c r="F9" s="169">
+      <c r="F9" s="164">
         <v>1</v>
       </c>
       <c r="G9" s="99">
@@ -6578,22 +6877,22 @@
       <c r="Q9" s="100"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10" s="194">
+      <c r="A10" s="183">
         <v>8</v>
       </c>
-      <c r="B10" s="195" t="s">
-        <v>131</v>
-      </c>
-      <c r="C10" s="205" t="s">
-        <v>147</v>
-      </c>
-      <c r="D10" s="205">
+      <c r="B10" s="184" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="194" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" s="194">
         <v>4</v>
       </c>
-      <c r="E10" s="196">
+      <c r="E10" s="185">
         <v>10</v>
       </c>
-      <c r="F10" s="169">
+      <c r="F10" s="164">
         <v>8</v>
       </c>
       <c r="G10" s="99">
@@ -6613,22 +6912,22 @@
       <c r="Q10" s="100"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11" s="194">
+      <c r="A11" s="183">
         <v>9</v>
       </c>
-      <c r="B11" s="195" t="s">
-        <v>132</v>
-      </c>
-      <c r="C11" s="205" t="s">
-        <v>147</v>
-      </c>
-      <c r="D11" s="205">
+      <c r="B11" s="184" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="194" t="s">
+        <v>145</v>
+      </c>
+      <c r="D11" s="194">
         <v>4</v>
       </c>
-      <c r="E11" s="196">
+      <c r="E11" s="185">
         <v>10</v>
       </c>
-      <c r="F11" s="169">
+      <c r="F11" s="164">
         <v>10</v>
       </c>
       <c r="G11" s="99">
@@ -6648,22 +6947,22 @@
       <c r="Q11" s="100"/>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A12" s="194">
+      <c r="A12" s="183">
         <v>10</v>
       </c>
-      <c r="B12" s="195" t="s">
-        <v>133</v>
-      </c>
-      <c r="C12" s="205" t="s">
-        <v>147</v>
-      </c>
-      <c r="D12" s="205">
+      <c r="B12" s="184" t="s">
+        <v>131</v>
+      </c>
+      <c r="C12" s="194" t="s">
+        <v>145</v>
+      </c>
+      <c r="D12" s="194">
         <v>4</v>
       </c>
-      <c r="E12" s="196">
+      <c r="E12" s="185">
         <v>10</v>
       </c>
-      <c r="F12" s="169">
+      <c r="F12" s="164">
         <v>10</v>
       </c>
       <c r="G12" s="99">
@@ -6683,22 +6982,22 @@
       <c r="Q12" s="100"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A13" s="194">
+      <c r="A13" s="183">
         <v>11</v>
       </c>
-      <c r="B13" s="195" t="s">
-        <v>134</v>
-      </c>
-      <c r="C13" s="205" t="s">
-        <v>147</v>
-      </c>
-      <c r="D13" s="205">
+      <c r="B13" s="184" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="194" t="s">
+        <v>145</v>
+      </c>
+      <c r="D13" s="194">
         <v>5</v>
       </c>
-      <c r="E13" s="196">
+      <c r="E13" s="185">
         <v>20</v>
       </c>
-      <c r="F13" s="169">
+      <c r="F13" s="164">
         <v>20</v>
       </c>
       <c r="G13" s="99">
@@ -6718,22 +7017,22 @@
       <c r="Q13" s="100"/>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A14" s="194">
+      <c r="A14" s="183">
         <v>12</v>
       </c>
-      <c r="B14" s="195" t="s">
-        <v>150</v>
-      </c>
-      <c r="C14" s="205" t="s">
-        <v>126</v>
-      </c>
-      <c r="D14" s="205">
+      <c r="B14" s="184" t="s">
+        <v>148</v>
+      </c>
+      <c r="C14" s="194" t="s">
+        <v>124</v>
+      </c>
+      <c r="D14" s="194">
         <v>3</v>
       </c>
-      <c r="E14" s="196">
+      <c r="E14" s="185">
         <v>2</v>
       </c>
-      <c r="F14" s="169">
+      <c r="F14" s="164">
         <v>2</v>
       </c>
       <c r="G14" s="99">
@@ -6753,22 +7052,22 @@
       <c r="Q14" s="100"/>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="194">
+      <c r="A15" s="183">
         <v>13</v>
       </c>
-      <c r="B15" s="195" t="s">
-        <v>135</v>
-      </c>
-      <c r="C15" s="205" t="s">
-        <v>150</v>
-      </c>
-      <c r="D15" s="205">
+      <c r="B15" s="184" t="s">
+        <v>133</v>
+      </c>
+      <c r="C15" s="194" t="s">
+        <v>148</v>
+      </c>
+      <c r="D15" s="194">
         <v>4</v>
       </c>
-      <c r="E15" s="196">
+      <c r="E15" s="185">
         <v>50</v>
       </c>
-      <c r="F15" s="169">
+      <c r="F15" s="164">
         <v>46</v>
       </c>
       <c r="G15" s="99">
@@ -6788,22 +7087,22 @@
       <c r="Q15" s="100"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A16" s="194">
+      <c r="A16" s="183">
         <v>14</v>
       </c>
-      <c r="B16" s="208" t="s">
-        <v>151</v>
-      </c>
-      <c r="C16" s="209" t="s">
-        <v>126</v>
-      </c>
-      <c r="D16" s="209">
+      <c r="B16" s="197" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="198" t="s">
+        <v>124</v>
+      </c>
+      <c r="D16" s="198">
         <v>3</v>
       </c>
-      <c r="E16" s="210">
+      <c r="E16" s="199">
         <v>4</v>
       </c>
-      <c r="F16" s="211">
+      <c r="F16" s="200">
         <v>4</v>
       </c>
       <c r="G16" s="104">
@@ -6823,22 +7122,22 @@
       <c r="Q16" s="105"/>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A17" s="194">
+      <c r="A17" s="183">
         <v>15</v>
       </c>
-      <c r="B17" s="197" t="s">
-        <v>136</v>
-      </c>
-      <c r="C17" s="206" t="s">
-        <v>150</v>
-      </c>
-      <c r="D17" s="206">
+      <c r="B17" s="186" t="s">
+        <v>134</v>
+      </c>
+      <c r="C17" s="195" t="s">
+        <v>148</v>
+      </c>
+      <c r="D17" s="195">
         <v>4</v>
       </c>
-      <c r="E17" s="198">
+      <c r="E17" s="187">
         <v>50</v>
       </c>
-      <c r="F17" s="199">
+      <c r="F17" s="188">
         <v>47</v>
       </c>
       <c r="G17" s="114">
@@ -6858,17 +7157,17 @@
       <c r="Q17" s="116"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A18" s="229"/>
-      <c r="B18" s="230" t="s">
-        <v>153</v>
-      </c>
-      <c r="C18" s="229" t="s">
+      <c r="A18" s="212"/>
+      <c r="B18" s="213" t="s">
         <v>151</v>
       </c>
-      <c r="D18" s="229">
+      <c r="C18" s="212" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" s="212">
         <v>5</v>
       </c>
-      <c r="E18" s="231">
+      <c r="E18" s="214">
         <v>0</v>
       </c>
       <c r="F18" s="10">
@@ -6882,61 +7181,61 @@
       </c>
     </row>
     <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A19" s="200"/>
-      <c r="B19" s="201" t="s">
+      <c r="A19" s="189"/>
+      <c r="B19" s="190" t="s">
         <v>37</v>
       </c>
-      <c r="C19" s="207"/>
-      <c r="D19" s="207"/>
-      <c r="E19" s="200">
+      <c r="C19" s="196"/>
+      <c r="D19" s="196"/>
+      <c r="E19" s="189">
         <f>SUM(E3:E18)</f>
         <v>166</v>
       </c>
-      <c r="F19" s="200">
+      <c r="F19" s="189">
         <f t="shared" ref="F19:Q19" si="0">SUM(F3:F17)</f>
         <v>158</v>
       </c>
-      <c r="G19" s="200">
+      <c r="G19" s="189">
         <f t="shared" si="0"/>
         <v>155</v>
       </c>
-      <c r="H19" s="200">
+      <c r="H19" s="189">
         <f t="shared" si="0"/>
         <v>161</v>
       </c>
-      <c r="I19" s="200">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="J19" s="200">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K19" s="200">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="L19" s="200">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="M19" s="200">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="N19" s="200">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="O19" s="200">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="P19" s="200">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="Q19" s="200">
+      <c r="I19" s="189">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="J19" s="189">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K19" s="189">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="L19" s="189">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="M19" s="189">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="N19" s="189">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="O19" s="189">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="P19" s="189">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="Q19" s="189">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
@@ -6979,15 +7278,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="258" t="s">
+      <c r="A1" s="263" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="259"/>
-      <c r="C1" s="259"/>
-      <c r="D1" s="259"/>
-      <c r="E1" s="259"/>
-      <c r="F1" s="259"/>
-      <c r="G1" s="260"/>
+      <c r="B1" s="264"/>
+      <c r="C1" s="264"/>
+      <c r="D1" s="264"/>
+      <c r="E1" s="264"/>
+      <c r="F1" s="264"/>
+      <c r="G1" s="265"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="138" t="s">
@@ -7013,7 +7312,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="255">
+      <c r="A3" s="260">
         <v>45658</v>
       </c>
       <c r="B3" s="123" t="s">
@@ -7037,7 +7336,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="256"/>
+      <c r="A4" s="261"/>
       <c r="B4" s="51" t="s">
         <v>74</v>
       </c>
@@ -7057,7 +7356,7 @@
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="257"/>
+      <c r="A5" s="262"/>
       <c r="B5" s="52" t="s">
         <v>76</v>
       </c>
@@ -7077,7 +7376,7 @@
       <c r="G5" s="13"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="255">
+      <c r="A6" s="260">
         <v>45689</v>
       </c>
       <c r="B6" s="123" t="s">
@@ -7102,7 +7401,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="256"/>
+      <c r="A7" s="261"/>
       <c r="B7" s="51" t="s">
         <v>74</v>
       </c>
@@ -7123,7 +7422,7 @@
       <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="257"/>
+      <c r="A8" s="262"/>
       <c r="B8" s="52" t="s">
         <v>76</v>
       </c>
@@ -7144,7 +7443,7 @@
       <c r="G8" s="13"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="255">
+      <c r="A9" s="260">
         <v>45717</v>
       </c>
       <c r="B9" s="123" t="s">
@@ -7165,7 +7464,7 @@
       <c r="G9" s="126"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="256"/>
+      <c r="A10" s="261"/>
       <c r="B10" s="51" t="s">
         <v>74</v>
       </c>
@@ -7184,7 +7483,7 @@
       <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="257"/>
+      <c r="A11" s="262"/>
       <c r="B11" s="52" t="s">
         <v>76</v>
       </c>
@@ -7203,7 +7502,7 @@
       <c r="G11" s="13"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="255">
+      <c r="A12" s="260">
         <v>45748</v>
       </c>
       <c r="B12" s="123" t="s">
@@ -7224,7 +7523,7 @@
       <c r="G12" s="126"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="256"/>
+      <c r="A13" s="261"/>
       <c r="B13" s="51" t="s">
         <v>74</v>
       </c>
@@ -7243,7 +7542,7 @@
       <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="257"/>
+      <c r="A14" s="262"/>
       <c r="B14" s="52" t="s">
         <v>76</v>
       </c>
@@ -7262,7 +7561,7 @@
       <c r="G14" s="13"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="255">
+      <c r="A15" s="260">
         <v>45778</v>
       </c>
       <c r="B15" s="123" t="s">
@@ -7283,7 +7582,7 @@
       <c r="G15" s="126"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="256"/>
+      <c r="A16" s="261"/>
       <c r="B16" s="51" t="s">
         <v>74</v>
       </c>
@@ -7302,7 +7601,7 @@
       <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="257"/>
+      <c r="A17" s="262"/>
       <c r="B17" s="52" t="s">
         <v>76</v>
       </c>
@@ -7321,7 +7620,7 @@
       <c r="G17" s="13"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="255">
+      <c r="A18" s="260">
         <v>45809</v>
       </c>
       <c r="B18" s="123" t="s">
@@ -7342,7 +7641,7 @@
       <c r="G18" s="126"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="256"/>
+      <c r="A19" s="261"/>
       <c r="B19" s="51" t="s">
         <v>74</v>
       </c>
@@ -7361,7 +7660,7 @@
       <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="257"/>
+      <c r="A20" s="262"/>
       <c r="B20" s="52" t="s">
         <v>76</v>
       </c>
@@ -7380,7 +7679,7 @@
       <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="255">
+      <c r="A21" s="260">
         <v>45839</v>
       </c>
       <c r="B21" s="123" t="s">
@@ -7401,7 +7700,7 @@
       <c r="G21" s="126"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="256"/>
+      <c r="A22" s="261"/>
       <c r="B22" s="51" t="s">
         <v>74</v>
       </c>
@@ -7420,7 +7719,7 @@
       <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="257"/>
+      <c r="A23" s="262"/>
       <c r="B23" s="52" t="s">
         <v>76</v>
       </c>
@@ -7439,7 +7738,7 @@
       <c r="G23" s="13"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="255">
+      <c r="A24" s="260">
         <v>45870</v>
       </c>
       <c r="B24" s="123" t="s">
@@ -7460,7 +7759,7 @@
       <c r="G24" s="126"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="256"/>
+      <c r="A25" s="261"/>
       <c r="B25" s="51" t="s">
         <v>74</v>
       </c>
@@ -7479,7 +7778,7 @@
       <c r="G25" s="12"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="257"/>
+      <c r="A26" s="262"/>
       <c r="B26" s="52" t="s">
         <v>76</v>
       </c>
@@ -7498,7 +7797,7 @@
       <c r="G26" s="13"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="255">
+      <c r="A27" s="260">
         <v>45901</v>
       </c>
       <c r="B27" s="123" t="s">
@@ -7519,7 +7818,7 @@
       <c r="G27" s="126"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="256"/>
+      <c r="A28" s="261"/>
       <c r="B28" s="51" t="s">
         <v>74</v>
       </c>
@@ -7538,7 +7837,7 @@
       <c r="G28" s="12"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="257"/>
+      <c r="A29" s="262"/>
       <c r="B29" s="52" t="s">
         <v>76</v>
       </c>
@@ -7557,7 +7856,7 @@
       <c r="G29" s="13"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="255">
+      <c r="A30" s="260">
         <v>45931</v>
       </c>
       <c r="B30" s="123" t="s">
@@ -7578,7 +7877,7 @@
       <c r="G30" s="126"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="256"/>
+      <c r="A31" s="261"/>
       <c r="B31" s="51" t="s">
         <v>74</v>
       </c>
@@ -7597,7 +7896,7 @@
       <c r="G31" s="12"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="257"/>
+      <c r="A32" s="262"/>
       <c r="B32" s="52" t="s">
         <v>76</v>
       </c>
@@ -7616,7 +7915,7 @@
       <c r="G32" s="13"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="255">
+      <c r="A33" s="260">
         <v>45962</v>
       </c>
       <c r="B33" s="123" t="s">
@@ -7637,7 +7936,7 @@
       <c r="G33" s="126"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="256"/>
+      <c r="A34" s="261"/>
       <c r="B34" s="51" t="s">
         <v>74</v>
       </c>
@@ -7656,7 +7955,7 @@
       <c r="G34" s="12"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="257"/>
+      <c r="A35" s="262"/>
       <c r="B35" s="52" t="s">
         <v>76</v>
       </c>
@@ -7675,7 +7974,7 @@
       <c r="G35" s="13"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="255">
+      <c r="A36" s="260">
         <v>45992</v>
       </c>
       <c r="B36" s="123" t="s">
@@ -7696,7 +7995,7 @@
       <c r="G36" s="126"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="256"/>
+      <c r="A37" s="261"/>
       <c r="B37" s="51" t="s">
         <v>74</v>
       </c>
@@ -7715,7 +8014,7 @@
       <c r="G37" s="12"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="257"/>
+      <c r="A38" s="262"/>
       <c r="B38" s="52" t="s">
         <v>76</v>
       </c>
@@ -7751,18 +8050,18 @@
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="E3:E38">
-    <cfRule type="expression" dxfId="7" priority="1">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>IF($F3="Not Met",TRUE, FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="8" priority="2">
       <formula>IF($F3="Met", TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F38">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
       <formula>"Met"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="equal">
       <formula>"Not Met"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7773,11 +8072,11 @@
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26BD38D1-9B67-480F-BC4F-1A3F2ECFC193}">
   <sheetPr>
-    <tabColor rgb="FFFF00FF"/>
+    <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6:C6"/>
     </sheetView>
   </sheetViews>
@@ -7792,15 +8091,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="261" t="s">
-        <v>155</v>
-      </c>
-      <c r="B1" s="262"/>
-      <c r="C1" s="262"/>
-      <c r="D1" s="262"/>
-      <c r="E1" s="262"/>
-      <c r="F1" s="263"/>
-      <c r="G1" s="264"/>
+      <c r="A1" s="266" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="267"/>
+      <c r="C1" s="267"/>
+      <c r="D1" s="267"/>
+      <c r="E1" s="267"/>
+      <c r="F1" s="268"/>
+      <c r="G1" s="269"/>
     </row>
     <row r="2" spans="1:7" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A2" s="145" t="s">
@@ -7810,7 +8109,7 @@
         <v>53</v>
       </c>
       <c r="C2" s="146" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D2" s="147" t="s">
         <v>54</v>
@@ -8088,18 +8387,18 @@
     <mergeCell ref="A1:G1"/>
   </mergeCells>
   <conditionalFormatting sqref="D3:D14">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>IF($F3="Above Target", TRUE, FALSE)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>IF($F3="Below Target",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F3:F14">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"Above Target"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
       <formula>"Below Target"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8110,12 +8409,12 @@
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18BC70EB-C584-4343-B833-809ED5B062E1}">
   <sheetPr>
-    <tabColor rgb="FFFF00FF"/>
+    <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:E15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="A1:E15"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8126,13 +8425,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="265" t="s">
+      <c r="A1" s="270" t="s">
         <v>64</v>
       </c>
-      <c r="B1" s="266"/>
-      <c r="C1" s="266"/>
-      <c r="D1" s="266"/>
-      <c r="E1" s="267"/>
+      <c r="B1" s="271"/>
+      <c r="C1" s="271"/>
+      <c r="D1" s="271"/>
+      <c r="E1" s="272"/>
     </row>
     <row r="2" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="118" t="s">

</xml_diff>

<commit_message>
added Excel Download / Upload
</commit_message>
<xml_diff>
--- a/public/Project Performance Template.xlsx
+++ b/public/Project Performance Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yahya Chaker\OneDrive\Desktop\Project Performance Review - 01\business-dashboard\business-dashboard\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yahya Chaker\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{082976B0-418E-4AF4-A56B-DEE3458133CE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A51EE95-B0A5-49BD-B852-88DD29D617A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="805" activeTab="1" xr2:uid="{23CBEA3F-BC00-4514-8C1F-F15676C82A9D}"/>
   </bookViews>
@@ -2544,6 +2544,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="17" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2553,15 +2562,6 @@
     <xf numFmtId="17" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2592,26 +2592,26 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3772,25 +3772,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="278" t="s">
+      <c r="A1" s="287" t="s">
         <v>159</v>
       </c>
-      <c r="B1" s="278"/>
-      <c r="C1" s="278"/>
-      <c r="D1" s="278"/>
-      <c r="E1" s="278"/>
-      <c r="F1" s="278"/>
-      <c r="G1" s="278"/>
-      <c r="H1" s="278"/>
-      <c r="I1" s="278"/>
-      <c r="J1" s="278"/>
-      <c r="K1" s="278"/>
+      <c r="B1" s="287"/>
+      <c r="C1" s="287"/>
+      <c r="D1" s="287"/>
+      <c r="E1" s="287"/>
+      <c r="F1" s="287"/>
+      <c r="G1" s="287"/>
+      <c r="H1" s="287"/>
+      <c r="I1" s="287"/>
+      <c r="J1" s="287"/>
+      <c r="K1" s="287"/>
     </row>
     <row r="2" spans="1:11" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="281" t="s">
+      <c r="A2" s="290" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="282"/>
+      <c r="B2" s="291"/>
       <c r="C2" s="219" t="str" cm="1">
         <f t="array" ref="C2:J2">TRANSPOSE(_xlfn._xlws.FILTER(Services!$B$3:$B$17,Services!$C$3:$C$17="Subcontractor"))</f>
         <v>System 8</v>
@@ -3816,15 +3816,15 @@
       <c r="J2" s="220" t="str">
         <v>System 15</v>
       </c>
-      <c r="K2" s="279" t="s">
+      <c r="K2" s="288" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="283" t="s">
+      <c r="A3" s="280" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="284"/>
+      <c r="B3" s="281"/>
       <c r="C3" s="165" t="str">
         <f>_xlfn.XLOOKUP(C2,Services!$B$3:$B$17,Services!$D$3:$D$17)</f>
         <v>Subcon-01</v>
@@ -3857,13 +3857,13 @@
         <f>_xlfn.XLOOKUP(J2,Services!$B$3:$B$17,Services!$D$3:$D$17)</f>
         <v>0</v>
       </c>
-      <c r="K3" s="280"/>
+      <c r="K3" s="289"/>
     </row>
     <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="291" t="s">
+      <c r="A4" s="286" t="s">
         <v>155</v>
       </c>
-      <c r="B4" s="283"/>
+      <c r="B4" s="280"/>
       <c r="C4" s="224">
         <v>1300000</v>
       </c>
@@ -3891,10 +3891,10 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="285" t="s">
+      <c r="A5" s="282" t="s">
         <v>154</v>
       </c>
-      <c r="B5" s="286"/>
+      <c r="B5" s="283"/>
       <c r="C5" s="168">
         <f>_xlfn.XLOOKUP(C2,Services!$B$3:$B$17,Services!$H$3:$H$17)</f>
         <v>1500000</v>
@@ -3933,10 +3933,10 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="287" t="s">
+      <c r="A6" s="278" t="s">
         <v>112</v>
       </c>
-      <c r="B6" s="288"/>
+      <c r="B6" s="279"/>
       <c r="C6" s="169">
         <f>IF(C3&gt;0,_xlfn.XLOOKUP(C2,Services!$B$3:$B$17,Services!$F$3:$F$17),"")</f>
         <v>45413</v>
@@ -3972,10 +3972,10 @@
       <c r="K6" s="208"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="283" t="s">
+      <c r="A7" s="280" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="284"/>
+      <c r="B7" s="281"/>
       <c r="C7" s="171">
         <f>IF(C3&gt;0,_xlfn.XLOOKUP(C2,Services!$B$3:$B$17,Services!$G$3:$G$17),"")</f>
         <v>46172</v>
@@ -4011,10 +4011,10 @@
       <c r="K7" s="209"/>
     </row>
     <row r="8" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="285" t="s">
+      <c r="A8" s="282" t="s">
         <v>115</v>
       </c>
-      <c r="B8" s="286"/>
+      <c r="B8" s="283"/>
       <c r="C8" s="167">
         <f>IF(C3&gt;0,DATEDIF(C6,C7,"M"),0)</f>
         <v>24</v>
@@ -4050,10 +4050,10 @@
       <c r="K8" s="210"/>
     </row>
     <row r="9" spans="1:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="289" t="s">
+      <c r="A9" s="284" t="s">
         <v>116</v>
       </c>
-      <c r="B9" s="290"/>
+      <c r="B9" s="285"/>
       <c r="C9" s="221">
         <f>IF(C8&lt;&gt;0,C5/C8,0)</f>
         <v>62500</v>
@@ -4106,16 +4106,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A5:B5"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B7"/>
     <mergeCell ref="A8:B8"/>
     <mergeCell ref="A9:B9"/>
     <mergeCell ref="A4:B4"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A5:B5"/>
   </mergeCells>
   <conditionalFormatting sqref="C5:K5">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
@@ -4792,7 +4792,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4983,7 +4983,7 @@
         <v>0.22596425925925917</v>
       </c>
       <c r="H5" s="36">
-        <v>3</v>
+        <v>33</v>
       </c>
       <c r="I5" s="48">
         <v>5000000</v>
@@ -5335,7 +5335,7 @@
       </c>
       <c r="H15" s="59">
         <f>SUM(H3:H14)</f>
-        <v>6</v>
+        <v>36</v>
       </c>
       <c r="I15" s="60">
         <f>SUM(I3:I14)</f>
@@ -7280,15 +7280,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="265" t="s">
+      <c r="A1" s="262" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="266"/>
-      <c r="C1" s="266"/>
-      <c r="D1" s="266"/>
-      <c r="E1" s="266"/>
-      <c r="F1" s="266"/>
-      <c r="G1" s="267"/>
+      <c r="B1" s="263"/>
+      <c r="C1" s="263"/>
+      <c r="D1" s="263"/>
+      <c r="E1" s="263"/>
+      <c r="F1" s="263"/>
+      <c r="G1" s="264"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="138" t="s">
@@ -7314,7 +7314,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="262">
+      <c r="A3" s="265">
         <v>45658</v>
       </c>
       <c r="B3" s="123" t="s">
@@ -7338,7 +7338,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="263"/>
+      <c r="A4" s="266"/>
       <c r="B4" s="51" t="s">
         <v>74</v>
       </c>
@@ -7358,7 +7358,7 @@
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="264"/>
+      <c r="A5" s="267"/>
       <c r="B5" s="52" t="s">
         <v>76</v>
       </c>
@@ -7378,7 +7378,7 @@
       <c r="G5" s="13"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="262">
+      <c r="A6" s="265">
         <v>45689</v>
       </c>
       <c r="B6" s="123" t="s">
@@ -7403,7 +7403,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="263"/>
+      <c r="A7" s="266"/>
       <c r="B7" s="51" t="s">
         <v>74</v>
       </c>
@@ -7424,7 +7424,7 @@
       <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="264"/>
+      <c r="A8" s="267"/>
       <c r="B8" s="52" t="s">
         <v>76</v>
       </c>
@@ -7445,7 +7445,7 @@
       <c r="G8" s="13"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="262">
+      <c r="A9" s="265">
         <v>45717</v>
       </c>
       <c r="B9" s="123" t="s">
@@ -7466,7 +7466,7 @@
       <c r="G9" s="126"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="263"/>
+      <c r="A10" s="266"/>
       <c r="B10" s="51" t="s">
         <v>74</v>
       </c>
@@ -7485,7 +7485,7 @@
       <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="264"/>
+      <c r="A11" s="267"/>
       <c r="B11" s="52" t="s">
         <v>76</v>
       </c>
@@ -7504,7 +7504,7 @@
       <c r="G11" s="13"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="262">
+      <c r="A12" s="265">
         <v>45748</v>
       </c>
       <c r="B12" s="123" t="s">
@@ -7525,7 +7525,7 @@
       <c r="G12" s="126"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="263"/>
+      <c r="A13" s="266"/>
       <c r="B13" s="51" t="s">
         <v>74</v>
       </c>
@@ -7544,7 +7544,7 @@
       <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="264"/>
+      <c r="A14" s="267"/>
       <c r="B14" s="52" t="s">
         <v>76</v>
       </c>
@@ -7563,7 +7563,7 @@
       <c r="G14" s="13"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="262">
+      <c r="A15" s="265">
         <v>45778</v>
       </c>
       <c r="B15" s="123" t="s">
@@ -7584,7 +7584,7 @@
       <c r="G15" s="126"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="263"/>
+      <c r="A16" s="266"/>
       <c r="B16" s="51" t="s">
         <v>74</v>
       </c>
@@ -7603,7 +7603,7 @@
       <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="264"/>
+      <c r="A17" s="267"/>
       <c r="B17" s="52" t="s">
         <v>76</v>
       </c>
@@ -7622,7 +7622,7 @@
       <c r="G17" s="13"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="262">
+      <c r="A18" s="265">
         <v>45809</v>
       </c>
       <c r="B18" s="123" t="s">
@@ -7643,7 +7643,7 @@
       <c r="G18" s="126"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="263"/>
+      <c r="A19" s="266"/>
       <c r="B19" s="51" t="s">
         <v>74</v>
       </c>
@@ -7662,7 +7662,7 @@
       <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="264"/>
+      <c r="A20" s="267"/>
       <c r="B20" s="52" t="s">
         <v>76</v>
       </c>
@@ -7681,7 +7681,7 @@
       <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="262">
+      <c r="A21" s="265">
         <v>45839</v>
       </c>
       <c r="B21" s="123" t="s">
@@ -7702,7 +7702,7 @@
       <c r="G21" s="126"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="263"/>
+      <c r="A22" s="266"/>
       <c r="B22" s="51" t="s">
         <v>74</v>
       </c>
@@ -7721,7 +7721,7 @@
       <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="264"/>
+      <c r="A23" s="267"/>
       <c r="B23" s="52" t="s">
         <v>76</v>
       </c>
@@ -7740,7 +7740,7 @@
       <c r="G23" s="13"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="262">
+      <c r="A24" s="265">
         <v>45870</v>
       </c>
       <c r="B24" s="123" t="s">
@@ -7761,7 +7761,7 @@
       <c r="G24" s="126"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="263"/>
+      <c r="A25" s="266"/>
       <c r="B25" s="51" t="s">
         <v>74</v>
       </c>
@@ -7780,7 +7780,7 @@
       <c r="G25" s="12"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="264"/>
+      <c r="A26" s="267"/>
       <c r="B26" s="52" t="s">
         <v>76</v>
       </c>
@@ -7799,7 +7799,7 @@
       <c r="G26" s="13"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="262">
+      <c r="A27" s="265">
         <v>45901</v>
       </c>
       <c r="B27" s="123" t="s">
@@ -7820,7 +7820,7 @@
       <c r="G27" s="126"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="263"/>
+      <c r="A28" s="266"/>
       <c r="B28" s="51" t="s">
         <v>74</v>
       </c>
@@ -7839,7 +7839,7 @@
       <c r="G28" s="12"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="264"/>
+      <c r="A29" s="267"/>
       <c r="B29" s="52" t="s">
         <v>76</v>
       </c>
@@ -7858,7 +7858,7 @@
       <c r="G29" s="13"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="262">
+      <c r="A30" s="265">
         <v>45931</v>
       </c>
       <c r="B30" s="123" t="s">
@@ -7879,7 +7879,7 @@
       <c r="G30" s="126"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="263"/>
+      <c r="A31" s="266"/>
       <c r="B31" s="51" t="s">
         <v>74</v>
       </c>
@@ -7898,7 +7898,7 @@
       <c r="G31" s="12"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="264"/>
+      <c r="A32" s="267"/>
       <c r="B32" s="52" t="s">
         <v>76</v>
       </c>
@@ -7917,7 +7917,7 @@
       <c r="G32" s="13"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="262">
+      <c r="A33" s="265">
         <v>45962</v>
       </c>
       <c r="B33" s="123" t="s">
@@ -7938,7 +7938,7 @@
       <c r="G33" s="126"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="263"/>
+      <c r="A34" s="266"/>
       <c r="B34" s="51" t="s">
         <v>74</v>
       </c>
@@ -7957,7 +7957,7 @@
       <c r="G34" s="12"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="264"/>
+      <c r="A35" s="267"/>
       <c r="B35" s="52" t="s">
         <v>76</v>
       </c>
@@ -7976,7 +7976,7 @@
       <c r="G35" s="13"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="262">
+      <c r="A36" s="265">
         <v>45992</v>
       </c>
       <c r="B36" s="123" t="s">
@@ -7997,7 +7997,7 @@
       <c r="G36" s="126"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="263"/>
+      <c r="A37" s="266"/>
       <c r="B37" s="51" t="s">
         <v>74</v>
       </c>
@@ -8016,7 +8016,7 @@
       <c r="G37" s="12"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="264"/>
+      <c r="A38" s="267"/>
       <c r="B38" s="52" t="s">
         <v>76</v>
       </c>
@@ -8036,11 +8036,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A30:A32"/>
     <mergeCell ref="A33:A35"/>
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="A3:A5"/>
@@ -8049,6 +8044,11 @@
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A18:A20"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A30:A32"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="E3:E38">

</xml_diff>

<commit_message>
added Excel Download / Upload-rev01
</commit_message>
<xml_diff>
--- a/public/Project Performance Template.xlsx
+++ b/public/Project Performance Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yahya Chaker\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A51EE95-B0A5-49BD-B852-88DD29D617A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F57A13-D47C-4260-9D04-2ADA7527B88D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="805" activeTab="1" xr2:uid="{23CBEA3F-BC00-4514-8C1F-F15676C82A9D}"/>
   </bookViews>
@@ -2544,6 +2544,15 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="73" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="17" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2553,15 +2562,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="17" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="3" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="3" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2592,26 +2592,26 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="55" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="57" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="59" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="86" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="87" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="92" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="85" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="74" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="82" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="83" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -3772,25 +3772,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="21" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="287" t="s">
+      <c r="A1" s="278" t="s">
         <v>159</v>
       </c>
-      <c r="B1" s="287"/>
-      <c r="C1" s="287"/>
-      <c r="D1" s="287"/>
-      <c r="E1" s="287"/>
-      <c r="F1" s="287"/>
-      <c r="G1" s="287"/>
-      <c r="H1" s="287"/>
-      <c r="I1" s="287"/>
-      <c r="J1" s="287"/>
-      <c r="K1" s="287"/>
+      <c r="B1" s="278"/>
+      <c r="C1" s="278"/>
+      <c r="D1" s="278"/>
+      <c r="E1" s="278"/>
+      <c r="F1" s="278"/>
+      <c r="G1" s="278"/>
+      <c r="H1" s="278"/>
+      <c r="I1" s="278"/>
+      <c r="J1" s="278"/>
+      <c r="K1" s="278"/>
     </row>
     <row r="2" spans="1:11" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="290" t="s">
+      <c r="A2" s="281" t="s">
         <v>113</v>
       </c>
-      <c r="B2" s="291"/>
+      <c r="B2" s="282"/>
       <c r="C2" s="219" t="str" cm="1">
         <f t="array" ref="C2:J2">TRANSPOSE(_xlfn._xlws.FILTER(Services!$B$3:$B$17,Services!$C$3:$C$17="Subcontractor"))</f>
         <v>System 8</v>
@@ -3816,15 +3816,15 @@
       <c r="J2" s="220" t="str">
         <v>System 15</v>
       </c>
-      <c r="K2" s="288" t="s">
+      <c r="K2" s="279" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="280" t="s">
+      <c r="A3" s="283" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="281"/>
+      <c r="B3" s="284"/>
       <c r="C3" s="165" t="str">
         <f>_xlfn.XLOOKUP(C2,Services!$B$3:$B$17,Services!$D$3:$D$17)</f>
         <v>Subcon-01</v>
@@ -3857,13 +3857,13 @@
         <f>_xlfn.XLOOKUP(J2,Services!$B$3:$B$17,Services!$D$3:$D$17)</f>
         <v>0</v>
       </c>
-      <c r="K3" s="289"/>
+      <c r="K3" s="280"/>
     </row>
     <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="286" t="s">
+      <c r="A4" s="291" t="s">
         <v>155</v>
       </c>
-      <c r="B4" s="280"/>
+      <c r="B4" s="283"/>
       <c r="C4" s="224">
         <v>1300000</v>
       </c>
@@ -3891,10 +3891,10 @@
       </c>
     </row>
     <row r="5" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="282" t="s">
+      <c r="A5" s="285" t="s">
         <v>154</v>
       </c>
-      <c r="B5" s="283"/>
+      <c r="B5" s="286"/>
       <c r="C5" s="168">
         <f>_xlfn.XLOOKUP(C2,Services!$B$3:$B$17,Services!$H$3:$H$17)</f>
         <v>1500000</v>
@@ -3933,10 +3933,10 @@
       </c>
     </row>
     <row r="6" spans="1:11" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="278" t="s">
+      <c r="A6" s="287" t="s">
         <v>112</v>
       </c>
-      <c r="B6" s="279"/>
+      <c r="B6" s="288"/>
       <c r="C6" s="169">
         <f>IF(C3&gt;0,_xlfn.XLOOKUP(C2,Services!$B$3:$B$17,Services!$F$3:$F$17),"")</f>
         <v>45413</v>
@@ -3972,10 +3972,10 @@
       <c r="K6" s="208"/>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="280" t="s">
+      <c r="A7" s="283" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="281"/>
+      <c r="B7" s="284"/>
       <c r="C7" s="171">
         <f>IF(C3&gt;0,_xlfn.XLOOKUP(C2,Services!$B$3:$B$17,Services!$G$3:$G$17),"")</f>
         <v>46172</v>
@@ -4011,10 +4011,10 @@
       <c r="K7" s="209"/>
     </row>
     <row r="8" spans="1:11" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="282" t="s">
+      <c r="A8" s="285" t="s">
         <v>115</v>
       </c>
-      <c r="B8" s="283"/>
+      <c r="B8" s="286"/>
       <c r="C8" s="167">
         <f>IF(C3&gt;0,DATEDIF(C6,C7,"M"),0)</f>
         <v>24</v>
@@ -4050,10 +4050,10 @@
       <c r="K8" s="210"/>
     </row>
     <row r="9" spans="1:11" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="284" t="s">
+      <c r="A9" s="289" t="s">
         <v>116</v>
       </c>
-      <c r="B9" s="285"/>
+      <c r="B9" s="290"/>
       <c r="C9" s="221">
         <f>IF(C8&lt;&gt;0,C5/C8,0)</f>
         <v>62500</v>
@@ -4106,16 +4106,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A4:B4"/>
     <mergeCell ref="A1:K1"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A4:B4"/>
   </mergeCells>
   <conditionalFormatting sqref="C5:K5">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
@@ -4792,7 +4792,7 @@
   <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4983,7 +4983,7 @@
         <v>0.22596425925925917</v>
       </c>
       <c r="H5" s="36">
-        <v>33</v>
+        <v>5</v>
       </c>
       <c r="I5" s="48">
         <v>5000000</v>
@@ -5335,7 +5335,7 @@
       </c>
       <c r="H15" s="59">
         <f>SUM(H3:H14)</f>
-        <v>36</v>
+        <v>8</v>
       </c>
       <c r="I15" s="60">
         <f>SUM(I3:I14)</f>
@@ -7280,15 +7280,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="262" t="s">
+      <c r="A1" s="265" t="s">
         <v>79</v>
       </c>
-      <c r="B1" s="263"/>
-      <c r="C1" s="263"/>
-      <c r="D1" s="263"/>
-      <c r="E1" s="263"/>
-      <c r="F1" s="263"/>
-      <c r="G1" s="264"/>
+      <c r="B1" s="266"/>
+      <c r="C1" s="266"/>
+      <c r="D1" s="266"/>
+      <c r="E1" s="266"/>
+      <c r="F1" s="266"/>
+      <c r="G1" s="267"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="138" t="s">
@@ -7314,7 +7314,7 @@
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="265">
+      <c r="A3" s="262">
         <v>45658</v>
       </c>
       <c r="B3" s="123" t="s">
@@ -7338,7 +7338,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="266"/>
+      <c r="A4" s="263"/>
       <c r="B4" s="51" t="s">
         <v>74</v>
       </c>
@@ -7358,7 +7358,7 @@
       <c r="G4" s="12"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="267"/>
+      <c r="A5" s="264"/>
       <c r="B5" s="52" t="s">
         <v>76</v>
       </c>
@@ -7378,7 +7378,7 @@
       <c r="G5" s="13"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="265">
+      <c r="A6" s="262">
         <v>45689</v>
       </c>
       <c r="B6" s="123" t="s">
@@ -7403,7 +7403,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="266"/>
+      <c r="A7" s="263"/>
       <c r="B7" s="51" t="s">
         <v>74</v>
       </c>
@@ -7424,7 +7424,7 @@
       <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8" s="267"/>
+      <c r="A8" s="264"/>
       <c r="B8" s="52" t="s">
         <v>76</v>
       </c>
@@ -7445,7 +7445,7 @@
       <c r="G8" s="13"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9" s="265">
+      <c r="A9" s="262">
         <v>45717</v>
       </c>
       <c r="B9" s="123" t="s">
@@ -7466,7 +7466,7 @@
       <c r="G9" s="126"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="266"/>
+      <c r="A10" s="263"/>
       <c r="B10" s="51" t="s">
         <v>74</v>
       </c>
@@ -7485,7 +7485,7 @@
       <c r="G10" s="12"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="267"/>
+      <c r="A11" s="264"/>
       <c r="B11" s="52" t="s">
         <v>76</v>
       </c>
@@ -7504,7 +7504,7 @@
       <c r="G11" s="13"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="265">
+      <c r="A12" s="262">
         <v>45748</v>
       </c>
       <c r="B12" s="123" t="s">
@@ -7525,7 +7525,7 @@
       <c r="G12" s="126"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="266"/>
+      <c r="A13" s="263"/>
       <c r="B13" s="51" t="s">
         <v>74</v>
       </c>
@@ -7544,7 +7544,7 @@
       <c r="G13" s="12"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="267"/>
+      <c r="A14" s="264"/>
       <c r="B14" s="52" t="s">
         <v>76</v>
       </c>
@@ -7563,7 +7563,7 @@
       <c r="G14" s="13"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="265">
+      <c r="A15" s="262">
         <v>45778</v>
       </c>
       <c r="B15" s="123" t="s">
@@ -7584,7 +7584,7 @@
       <c r="G15" s="126"/>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A16" s="266"/>
+      <c r="A16" s="263"/>
       <c r="B16" s="51" t="s">
         <v>74</v>
       </c>
@@ -7603,7 +7603,7 @@
       <c r="G16" s="12"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" s="267"/>
+      <c r="A17" s="264"/>
       <c r="B17" s="52" t="s">
         <v>76</v>
       </c>
@@ -7622,7 +7622,7 @@
       <c r="G17" s="13"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" s="265">
+      <c r="A18" s="262">
         <v>45809</v>
       </c>
       <c r="B18" s="123" t="s">
@@ -7643,7 +7643,7 @@
       <c r="G18" s="126"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" s="266"/>
+      <c r="A19" s="263"/>
       <c r="B19" s="51" t="s">
         <v>74</v>
       </c>
@@ -7662,7 +7662,7 @@
       <c r="G19" s="12"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" s="267"/>
+      <c r="A20" s="264"/>
       <c r="B20" s="52" t="s">
         <v>76</v>
       </c>
@@ -7681,7 +7681,7 @@
       <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" s="265">
+      <c r="A21" s="262">
         <v>45839</v>
       </c>
       <c r="B21" s="123" t="s">
@@ -7702,7 +7702,7 @@
       <c r="G21" s="126"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" s="266"/>
+      <c r="A22" s="263"/>
       <c r="B22" s="51" t="s">
         <v>74</v>
       </c>
@@ -7721,7 +7721,7 @@
       <c r="G22" s="12"/>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A23" s="267"/>
+      <c r="A23" s="264"/>
       <c r="B23" s="52" t="s">
         <v>76</v>
       </c>
@@ -7740,7 +7740,7 @@
       <c r="G23" s="13"/>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A24" s="265">
+      <c r="A24" s="262">
         <v>45870</v>
       </c>
       <c r="B24" s="123" t="s">
@@ -7761,7 +7761,7 @@
       <c r="G24" s="126"/>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A25" s="266"/>
+      <c r="A25" s="263"/>
       <c r="B25" s="51" t="s">
         <v>74</v>
       </c>
@@ -7780,7 +7780,7 @@
       <c r="G25" s="12"/>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A26" s="267"/>
+      <c r="A26" s="264"/>
       <c r="B26" s="52" t="s">
         <v>76</v>
       </c>
@@ -7799,7 +7799,7 @@
       <c r="G26" s="13"/>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A27" s="265">
+      <c r="A27" s="262">
         <v>45901</v>
       </c>
       <c r="B27" s="123" t="s">
@@ -7820,7 +7820,7 @@
       <c r="G27" s="126"/>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A28" s="266"/>
+      <c r="A28" s="263"/>
       <c r="B28" s="51" t="s">
         <v>74</v>
       </c>
@@ -7839,7 +7839,7 @@
       <c r="G28" s="12"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A29" s="267"/>
+      <c r="A29" s="264"/>
       <c r="B29" s="52" t="s">
         <v>76</v>
       </c>
@@ -7858,7 +7858,7 @@
       <c r="G29" s="13"/>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A30" s="265">
+      <c r="A30" s="262">
         <v>45931</v>
       </c>
       <c r="B30" s="123" t="s">
@@ -7879,7 +7879,7 @@
       <c r="G30" s="126"/>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A31" s="266"/>
+      <c r="A31" s="263"/>
       <c r="B31" s="51" t="s">
         <v>74</v>
       </c>
@@ -7898,7 +7898,7 @@
       <c r="G31" s="12"/>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A32" s="267"/>
+      <c r="A32" s="264"/>
       <c r="B32" s="52" t="s">
         <v>76</v>
       </c>
@@ -7917,7 +7917,7 @@
       <c r="G32" s="13"/>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A33" s="265">
+      <c r="A33" s="262">
         <v>45962</v>
       </c>
       <c r="B33" s="123" t="s">
@@ -7938,7 +7938,7 @@
       <c r="G33" s="126"/>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A34" s="266"/>
+      <c r="A34" s="263"/>
       <c r="B34" s="51" t="s">
         <v>74</v>
       </c>
@@ -7957,7 +7957,7 @@
       <c r="G34" s="12"/>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A35" s="267"/>
+      <c r="A35" s="264"/>
       <c r="B35" s="52" t="s">
         <v>76</v>
       </c>
@@ -7976,7 +7976,7 @@
       <c r="G35" s="13"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A36" s="265">
+      <c r="A36" s="262">
         <v>45992</v>
       </c>
       <c r="B36" s="123" t="s">
@@ -7997,7 +7997,7 @@
       <c r="G36" s="126"/>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A37" s="266"/>
+      <c r="A37" s="263"/>
       <c r="B37" s="51" t="s">
         <v>74</v>
       </c>
@@ -8016,7 +8016,7 @@
       <c r="G37" s="12"/>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A38" s="267"/>
+      <c r="A38" s="264"/>
       <c r="B38" s="52" t="s">
         <v>76</v>
       </c>
@@ -8036,6 +8036,11 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A21:A23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="A27:A29"/>
+    <mergeCell ref="A30:A32"/>
     <mergeCell ref="A33:A35"/>
     <mergeCell ref="A36:A38"/>
     <mergeCell ref="A3:A5"/>
@@ -8044,11 +8049,6 @@
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A15:A17"/>
     <mergeCell ref="A18:A20"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A21:A23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="A27:A29"/>
-    <mergeCell ref="A30:A32"/>
   </mergeCells>
   <phoneticPr fontId="8" type="noConversion"/>
   <conditionalFormatting sqref="E3:E38">

</xml_diff>